<commit_message>
5 rounds of training - average out instability of SB-3 algos
</commit_message>
<xml_diff>
--- a/drawings_tables/LaTex_Table_Formatter.xlsx
+++ b/drawings_tables/LaTex_Table_Formatter.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rajesh\HEI\P-4 Research Phase\Article_Empirical_Study\drawings_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE32BA17-8898-4A20-8FFD-6C4ECCC127D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397AE2E7-E08C-4B33-9B90-58C853F8B112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="558" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="664" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Latex" sheetId="18" r:id="rId1"/>
-    <sheet name="SB-3_Stability_2k" sheetId="13" r:id="rId2"/>
-    <sheet name="SB-3_Stability_4k" sheetId="11" r:id="rId3"/>
-    <sheet name="Stability_10k-1" sheetId="16" r:id="rId4"/>
-    <sheet name="20K-colored" sheetId="19" r:id="rId5"/>
-    <sheet name="10K-colored" sheetId="20" r:id="rId6"/>
-    <sheet name="10K-Mono" sheetId="17" r:id="rId7"/>
+    <sheet name="Article tables" sheetId="21" r:id="rId2"/>
+    <sheet name="SB-3_Stability_2k" sheetId="13" r:id="rId3"/>
+    <sheet name="SB-3_Stability_4k" sheetId="11" r:id="rId4"/>
+    <sheet name="Stability_10k-1" sheetId="16" r:id="rId5"/>
+    <sheet name="20K-colored" sheetId="19" r:id="rId6"/>
+    <sheet name="10K-colored" sheetId="20" r:id="rId7"/>
+    <sheet name="10K-Mono" sheetId="17" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1182" uniqueCount="188">
   <si>
     <t>expt_n</t>
   </si>
@@ -1706,11 +1707,11 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="33" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="38" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3040,28 +3041,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40702C28-AEBD-47E7-8513-81FE413835A5}">
   <dimension ref="A2:S40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="T32" sqref="T32"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
-    <col min="3" max="5" width="6.7109375" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="6.7109375" customWidth="1"/>
-    <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="6.7109375" customWidth="1"/>
-    <col min="14" max="14" width="3.42578125" customWidth="1"/>
-    <col min="15" max="17" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+    <col min="3" max="5" width="6.6640625" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="6.6640625" customWidth="1"/>
+    <col min="10" max="10" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="6.6640625" customWidth="1"/>
+    <col min="14" max="14" width="3.44140625" customWidth="1"/>
+    <col min="15" max="17" width="6.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:19" ht="18" x14ac:dyDescent="0.35">
       <c r="B2" s="75" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:19" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>66</v>
       </c>
@@ -3079,7 +3080,7 @@
         <v xml:space="preserve"> &amp;REINFORCE &amp; &amp; &amp;  &amp;SB-3 A2C &amp; &amp; &amp; &amp;SB-3 DQN &amp; &amp; &amp; &amp;SB-3 PPO &amp; &amp;\\</v>
       </c>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>138</v>
       </c>
@@ -3124,7 +3125,7 @@
         <v>Model &amp;Precision &amp;Recall &amp;F1-score &amp;  &amp;Precision &amp;Recall &amp;F1-score &amp; &amp;Precision &amp;Recall &amp;F1-score &amp; &amp;Precision &amp;Recall &amp;F1-score\\</v>
       </c>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>157</v>
       </c>
@@ -3172,7 +3173,7 @@
         <v>Simulated  - No noise &amp;1.000 &amp;0.700 &amp;0.823 &amp;  &amp;0.487 &amp;0.440 &amp;0.460 &amp; &amp;0.067 &amp;0.010 &amp;0.017 &amp; &amp;0.457 &amp;0.280 &amp;0.343\\</v>
       </c>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>165</v>
       </c>
@@ -3220,7 +3221,7 @@
         <v>Simulated  - Low noise &amp;0.938 &amp;0.900 &amp;0.918 &amp;  &amp;0.000 &amp;0.000 &amp;0.000 &amp; &amp;0.450 &amp;0.030 &amp;0.055 &amp; &amp;0.367 &amp;0.060 &amp;0.103\\</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>166</v>
       </c>
@@ -3268,7 +3269,7 @@
         <v>Simulated  - High noise &amp;0.895 &amp;1.000 &amp;0.944 &amp;  &amp;0.498 &amp;0.530 &amp;0.511 &amp; &amp;0.497 &amp;0.960 &amp;0.655 &amp; &amp;0.584 &amp;0.150 &amp;0.237\\</v>
       </c>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>158</v>
       </c>
@@ -3316,7 +3317,7 @@
         <v>PHM C01 SS - No noise &amp;0.907 &amp;0.960 &amp;0.932 &amp;  &amp;0.523 &amp;0.560 &amp;0.538 &amp; &amp;0.367 &amp;0.030 &amp;0.055 &amp; &amp;0.498 &amp;0.250 &amp;0.332\\</v>
       </c>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>167</v>
       </c>
@@ -3364,7 +3365,7 @@
         <v>PHM C01 SS - Low noise &amp;0.886 &amp;0.800 &amp;0.836 &amp;  &amp;0.380 &amp;0.130 &amp;0.192 &amp; &amp;0.400 &amp;0.020 &amp;0.038 &amp; &amp;0.463 &amp;0.140 &amp;0.207\\</v>
       </c>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>168</v>
       </c>
@@ -3412,7 +3413,7 @@
         <v>PHM C01 SS - High noise &amp;0.783 &amp;0.930 &amp;0.849 &amp;  &amp;0.000 &amp;0.000 &amp;0.000 &amp; &amp;0.508 &amp;0.960 &amp;0.664 &amp; &amp;0.519 &amp;0.210 &amp;0.287\\</v>
       </c>
     </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>159</v>
       </c>
@@ -3460,7 +3461,7 @@
         <v>PHM C04 SS - No noise &amp;0.821 &amp;0.960 &amp;0.885 &amp;  &amp;0.513 &amp;0.090 &amp;0.149 &amp; &amp;0.497 &amp;0.970 &amp;0.657 &amp; &amp;0.489 &amp;0.470 &amp;0.478\\</v>
       </c>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>169</v>
       </c>
@@ -3508,7 +3509,7 @@
         <v>PHM C04 SS - Low noise &amp;0.739 &amp;0.990 &amp;0.846 &amp;  &amp;0.474 &amp;0.510 &amp;0.487 &amp; &amp;0.706 &amp;0.720 &amp;0.712 &amp; &amp;0.532 &amp;0.280 &amp;0.366\\</v>
       </c>
     </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>170</v>
       </c>
@@ -3556,7 +3557,7 @@
         <v>PHM C04 SS - High noise &amp;0.671 &amp;0.780 &amp;0.720 &amp;  &amp;0.522 &amp;0.550 &amp;0.534 &amp; &amp;0.500 &amp;0.980 &amp;0.662 &amp; &amp;0.472 &amp;0.250 &amp;0.325\\</v>
       </c>
     </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>160</v>
       </c>
@@ -3604,7 +3605,7 @@
         <v>PHM C06 SS - No noise &amp;1.000 &amp;0.650 &amp;0.785 &amp;  &amp;0.465 &amp;0.460 &amp;0.461 &amp; &amp;0.511 &amp;0.980 &amp;0.671 &amp; &amp;0.379 &amp;0.140 &amp;0.198\\</v>
       </c>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>171</v>
       </c>
@@ -3652,7 +3653,7 @@
         <v>PHM C06 SS - Low noise &amp;0.978 &amp;0.840 &amp;0.902 &amp;  &amp;0.493 &amp;0.530 &amp;0.508 &amp; &amp;0.951 &amp;0.580 &amp;0.720 &amp; &amp;0.500 &amp;0.380 &amp;0.432\\</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>172</v>
       </c>
@@ -3700,7 +3701,7 @@
         <v>PHM C06 SS - High noise &amp;0.715 &amp;0.880 &amp;0.789 &amp;  &amp;0.505 &amp;0.470 &amp;0.482 &amp; &amp;0.505 &amp;0.980 &amp;0.667 &amp; &amp;0.369 &amp;0.110 &amp;0.169\\</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>161</v>
       </c>
@@ -3748,7 +3749,7 @@
         <v>PHM C01 MS - No noise &amp;0.798 &amp;0.920 &amp;0.852 &amp;  &amp;0.514 &amp;0.590 &amp;0.549 &amp; &amp;0.584 &amp;0.970 &amp;0.729 &amp; &amp;0.486 &amp;0.240 &amp;0.313\\</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>162</v>
       </c>
@@ -3796,7 +3797,7 @@
         <v>PHM C04 MS - No noise &amp;0.774 &amp;0.690 &amp;0.728 &amp;  &amp;0.476 &amp;0.530 &amp;0.500 &amp; &amp;0.506 &amp;0.970 &amp;0.664 &amp; &amp;0.495 &amp;0.340 &amp;0.401\\</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>163</v>
       </c>
@@ -3844,15 +3845,15 @@
         <v>PHM C06 MS - No noise &amp;1.000 &amp;0.570 &amp;0.725 &amp;  &amp;0.491 &amp;0.600 &amp;0.536 &amp; &amp;0.492 &amp;0.960 &amp;0.651 &amp; &amp;0.446 &amp;0.480 &amp;0.460\\</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="B23" s="75" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="B24" s="75"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>175</v>
       </c>
@@ -3884,7 +3885,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B26" s="5"/>
       <c r="C26" s="5" t="s">
         <v>79</v>
@@ -3903,7 +3904,7 @@
         <v xml:space="preserve"> &amp;Precision &amp; &amp; &amp;Recall &amp; &amp; &amp;F1-score &amp; \\</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C27" s="6" t="s">
         <v>80</v>
       </c>
@@ -3927,115 +3928,123 @@
         <v xml:space="preserve"> &amp;Mean &amp;SD &amp; &amp;Mean &amp;SD &amp; &amp;Mean &amp;SD \\</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>63</v>
       </c>
       <c r="C28" s="3">
-        <v>0</v>
+        <v>0.42867705419544677</v>
       </c>
       <c r="D28" s="3">
-        <v>0</v>
-      </c>
-      <c r="F28" s="3">
-        <v>0</v>
+        <v>8.7531082407871122E-2</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1">
+        <v>0.41113725490196051</v>
       </c>
       <c r="G28" s="3">
-        <v>0</v>
-      </c>
+        <v>8.5377782913454964E-2</v>
+      </c>
+      <c r="H28" s="3"/>
       <c r="I28" s="3">
-        <v>0</v>
-      </c>
-      <c r="J28" s="3">
-        <v>0</v>
+        <v>0.40295044267970159</v>
+      </c>
+      <c r="J28" s="1">
+        <v>6.9888457830582507E-2</v>
       </c>
       <c r="L28" t="str">
         <f>_xlfn.CONCAT(B28, " &amp;", TEXT(C28, "0.000"), " &amp;", TEXT(D28, "0.000"), " &amp; &amp;",TEXT( F28,  "0.000"), " &amp;", TEXT(G28,  "0.000"), " &amp; &amp;", TEXT(I28,  "0.000"), " &amp;", TEXT(J28,  "0.000"), " \\")</f>
-        <v>A2C &amp;0.000 &amp;0.000 &amp; &amp;0.000 &amp;0.000 &amp; &amp;0.000 &amp;0.000 \\</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+        <v>A2C &amp;0.429 &amp;0.088 &amp; &amp;0.411 &amp;0.085 &amp; &amp;0.403 &amp;0.070 \\</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>64</v>
       </c>
       <c r="C29" s="3">
-        <v>0</v>
+        <v>0.52911107506627419</v>
       </c>
       <c r="D29" s="3">
-        <v>0</v>
-      </c>
-      <c r="F29" s="3">
-        <v>0</v>
+        <v>0.12067194028230305</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1">
+        <v>0.69262745098039225</v>
       </c>
       <c r="G29" s="3">
-        <v>0</v>
-      </c>
+        <v>3.4964787208832351E-2</v>
+      </c>
+      <c r="H29" s="3"/>
       <c r="I29" s="3">
-        <v>0</v>
-      </c>
-      <c r="J29" s="3">
-        <v>0</v>
+        <v>0.52090689324726325</v>
+      </c>
+      <c r="J29" s="1">
+        <v>2.805981213734909E-2</v>
       </c>
       <c r="L29" t="str">
         <f>_xlfn.CONCAT(B29, " &amp;", TEXT(C29, "0.000"), " &amp;", TEXT(D29, "0.000"), " &amp; &amp;",TEXT( F29,  "0.000"), " &amp;", TEXT(G29,  "0.000"), " &amp; &amp;", TEXT(I29,  "0.000"), " &amp;", TEXT(J29,  "0.000"), " \\")</f>
-        <v>DQN &amp;0.000 &amp;0.000 &amp; &amp;0.000 &amp;0.000 &amp; &amp;0.000 &amp;0.000 \\</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+        <v>DQN &amp;0.529 &amp;0.121 &amp; &amp;0.693 &amp;0.035 &amp; &amp;0.521 &amp;0.028 \\</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>65</v>
       </c>
       <c r="C30" s="3">
-        <v>0</v>
+        <v>0.47711924804775518</v>
       </c>
       <c r="D30" s="3">
-        <v>0</v>
-      </c>
-      <c r="F30" s="3">
-        <v>0</v>
+        <v>0.15319259899601673</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1">
+        <v>0.26541176470588207</v>
       </c>
       <c r="G30" s="3">
-        <v>0</v>
-      </c>
+        <v>8.9551591423027307E-2</v>
+      </c>
+      <c r="H30" s="3"/>
       <c r="I30" s="3">
-        <v>0</v>
-      </c>
-      <c r="J30" s="3">
-        <v>0</v>
+        <v>0.31990474837618449</v>
+      </c>
+      <c r="J30" s="1">
+        <v>0.10129818207014342</v>
       </c>
       <c r="L30" t="str">
         <f>_xlfn.CONCAT(B30, " &amp;", TEXT(C30, "0.000"), " &amp;", TEXT(D30, "0.000"), " &amp; &amp;",TEXT( F30,  "0.000"), " &amp;", TEXT(G30,  "0.000"), " &amp; &amp;", TEXT(I30,  "0.000"), " &amp;", TEXT(J30,  "0.000"), " \\")</f>
-        <v>PPO &amp;0.000 &amp;0.000 &amp; &amp;0.000 &amp;0.000 &amp; &amp;0.000 &amp;0.000 \\</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+        <v>PPO &amp;0.477 &amp;0.153 &amp; &amp;0.265 &amp;0.090 &amp; &amp;0.320 &amp;0.101 \\</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B31" s="12" t="s">
         <v>66</v>
       </c>
       <c r="C31" s="3">
-        <v>0</v>
+        <v>0.86870732223005609</v>
       </c>
       <c r="D31" s="3">
-        <v>0</v>
-      </c>
-      <c r="F31" s="3">
-        <v>0</v>
+        <v>3.8524356690436232E-2</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1">
+        <v>0.84752941176470575</v>
       </c>
       <c r="G31" s="3">
-        <v>0</v>
-      </c>
+        <v>6.1915357954097625E-2</v>
+      </c>
+      <c r="H31" s="3"/>
       <c r="I31" s="3">
-        <v>0</v>
-      </c>
-      <c r="J31" s="3">
-        <v>0</v>
+        <v>0.84200888071204683</v>
+      </c>
+      <c r="J31" s="1">
+        <v>4.4745355112257877E-2</v>
       </c>
       <c r="L31" t="str">
         <f>_xlfn.CONCAT(B31, " &amp;", TEXT(C31, "0.000"), " &amp;", TEXT(D31, "0.000"), " &amp; &amp;",TEXT( F31,  "0.000"), " &amp;", TEXT(G31,  "0.000"), " &amp; &amp;", TEXT(I31,  "0.000"), " &amp;", TEXT(J31,  "0.000"), " \\")</f>
-        <v>REINFORCE &amp;0.000 &amp;0.000 &amp; &amp;0.000 &amp;0.000 &amp; &amp;0.000 &amp;0.000 \\</v>
-      </c>
-    </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+        <v>REINFORCE &amp;0.869 &amp;0.039 &amp; &amp;0.848 &amp;0.062 &amp; &amp;0.842 &amp;0.045 \\</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B33">
         <v>1</v>
       </c>
@@ -4073,7 +4082,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B34" s="68" t="s">
         <v>176</v>
       </c>
@@ -4111,7 +4120,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B35" s="5"/>
       <c r="C35" s="5" t="s">
         <v>79</v>
@@ -4134,7 +4143,7 @@
         <v xml:space="preserve"> &amp;Precision &amp; &amp; &amp;Recall &amp; &amp; &amp;F1-score &amp;&amp; &amp;F-beta score (0.5) \\</v>
       </c>
     </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C36" s="6" t="s">
         <v>80</v>
       </c>
@@ -4164,7 +4173,7 @@
         <v xml:space="preserve"> &amp;Mean &amp;SD &amp; &amp;Mean &amp;SD &amp; &amp;Mean &amp;SD&amp; &amp;Mean \\</v>
       </c>
     </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>63</v>
       </c>
@@ -4197,7 +4206,7 @@
         <v>A2C &amp;1.000 &amp;2.000 &amp;  &amp;3.000 &amp;4.000 &amp; &amp; 5.000 &amp;6.000 &amp; &amp;7.000 &amp;8.000 \\</v>
       </c>
     </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>64</v>
       </c>
@@ -4230,7 +4239,7 @@
         <v>DQN &amp;1.000 &amp;2.000 &amp;  &amp;3.000 &amp;4.000 &amp; &amp; 5.000 &amp;6.000 &amp; &amp;7.000 &amp;8.000 \\</v>
       </c>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>65</v>
       </c>
@@ -4263,7 +4272,7 @@
         <v>PPO &amp;1.000 &amp;2.000 &amp;  &amp;3.000 &amp;4.000 &amp; &amp; 5.000 &amp;6.000 &amp; &amp;7.000 &amp;8.000 \\</v>
       </c>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B40" s="12" t="s">
         <v>66</v>
       </c>
@@ -4303,6 +4312,1280 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4999B83E-892B-4D36-92D7-B72E899E0B24}">
+  <dimension ref="A2:S40"/>
+  <sheetViews>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+    <col min="3" max="5" width="6.6640625" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="6.6640625" customWidth="1"/>
+    <col min="10" max="10" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="6.6640625" customWidth="1"/>
+    <col min="14" max="14" width="3.44140625" customWidth="1"/>
+    <col min="15" max="17" width="6.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:19" ht="18" x14ac:dyDescent="0.35">
+      <c r="B2" s="75" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" t="s">
+        <v>135</v>
+      </c>
+      <c r="K4" t="s">
+        <v>136</v>
+      </c>
+      <c r="O4" t="s">
+        <v>137</v>
+      </c>
+      <c r="S4" t="str">
+        <f>CONCATENATE(B4, " &amp;", C4," &amp;", D4," &amp;", E4," &amp; ", " &amp;", G4," &amp;", H4," &amp;", I4," &amp;", " &amp;", K4," &amp;", L4," &amp;", M4," &amp;", " &amp;", O4," &amp;", P4," &amp;", Q4,"\\")</f>
+        <v xml:space="preserve"> &amp;REINFORCE &amp; &amp; &amp;  &amp;SB-3 A2C &amp; &amp; &amp; &amp;SB-3 DQN &amp; &amp; &amp; &amp;SB-3 PPO &amp; &amp;\\</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I5" t="s">
+        <v>83</v>
+      </c>
+      <c r="K5" t="s">
+        <v>79</v>
+      </c>
+      <c r="L5" t="s">
+        <v>82</v>
+      </c>
+      <c r="M5" t="s">
+        <v>83</v>
+      </c>
+      <c r="O5" t="s">
+        <v>79</v>
+      </c>
+      <c r="P5" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>83</v>
+      </c>
+      <c r="S5" t="str">
+        <f>CONCATENATE(B5, " &amp;", TEXT(C5, "0.000")," &amp;", TEXT(D5, "0.000"), " &amp;", TEXT(E5, "0.000"), " &amp; ", " &amp;", TEXT(G5, "0.000")," &amp;", TEXT(H5, "0.000")," &amp;", TEXT(I5, "0.000")," &amp;", " &amp;", TEXT(K5, "0.000")," &amp;", TEXT(L5, "0.000")," &amp;", TEXT(M5, "0.000")," &amp;", " &amp;", TEXT(O5, "0.000")," &amp;", TEXT(P5, "0.000")," &amp;", TEXT(Q5, "0.000"),"\\")</f>
+        <v>Model &amp;Precision &amp;Recall &amp;F1-score &amp;  &amp;Precision &amp;Recall &amp;F1-score &amp; &amp;Precision &amp;Recall &amp;F1-score &amp; &amp;Precision &amp;Recall &amp;F1-score\\</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0.46</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="M6" s="1">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="P6" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="S6" t="str">
+        <f>CONCATENATE(B6, " &amp;", TEXT(C6, "0.000")," &amp;", TEXT(D6, "0.000"), " &amp;", TEXT(E6, "0.000"), " &amp; ", " &amp;", TEXT(G6, "0.000")," &amp;", TEXT(H6, "0.000")," &amp;", TEXT(I6, "0.000")," &amp;", " &amp;", TEXT(K6, "0.000")," &amp;", TEXT(L6, "0.000")," &amp;", TEXT(M6, "0.000")," &amp;", " &amp;", TEXT(O6, "0.000")," &amp;", TEXT(P6, "0.000")," &amp;", TEXT(Q6, "0.000"),"\\")</f>
+        <v>Simulated  - No noise &amp;1.000 &amp;0.700 &amp;0.823 &amp;  &amp;0.487 &amp;0.440 &amp;0.460 &amp; &amp;0.067 &amp;0.010 &amp;0.017 &amp; &amp;0.457 &amp;0.280 &amp;0.343\\</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="M7" s="1">
+        <v>5.5E-2</v>
+      </c>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="P7" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="S7" t="str">
+        <f t="shared" ref="S7:S20" si="0">CONCATENATE(B7, " &amp;", TEXT(C7, "0.000")," &amp;", TEXT(D7, "0.000"), " &amp;", TEXT(E7, "0.000"), " &amp; ", " &amp;", TEXT(G7, "0.000")," &amp;", TEXT(H7, "0.000")," &amp;", TEXT(I7, "0.000")," &amp;", " &amp;", TEXT(K7, "0.000")," &amp;", TEXT(L7, "0.000")," &amp;", TEXT(M7, "0.000")," &amp;", " &amp;", TEXT(O7, "0.000")," &amp;", TEXT(P7, "0.000")," &amp;", TEXT(Q7, "0.000"),"\\")</f>
+        <v>Simulated  - Low noise &amp;0.938 &amp;0.900 &amp;0.918 &amp;  &amp;0.000 &amp;0.000 &amp;0.000 &amp; &amp;0.450 &amp;0.030 &amp;0.055 &amp; &amp;0.367 &amp;0.060 &amp;0.103\\</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>166</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1">
+        <v>0.498</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0.51100000000000001</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1">
+        <v>0.497</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="M8" s="1">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1">
+        <v>0.58399999999999996</v>
+      </c>
+      <c r="P8" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>0.23699999999999999</v>
+      </c>
+      <c r="S8" t="str">
+        <f t="shared" si="0"/>
+        <v>Simulated  - High noise &amp;0.895 &amp;1.000 &amp;0.944 &amp;  &amp;0.498 &amp;0.530 &amp;0.511 &amp; &amp;0.497 &amp;0.960 &amp;0.655 &amp; &amp;0.584 &amp;0.150 &amp;0.237\\</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.90700000000000003</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1">
+        <v>0.52300000000000002</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="M9" s="1">
+        <v>5.5E-2</v>
+      </c>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1">
+        <v>0.498</v>
+      </c>
+      <c r="P9" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>0.33200000000000002</v>
+      </c>
+      <c r="S9" t="str">
+        <f t="shared" si="0"/>
+        <v>PHM C01 SS - No noise &amp;0.907 &amp;0.960 &amp;0.932 &amp;  &amp;0.523 &amp;0.560 &amp;0.538 &amp; &amp;0.367 &amp;0.030 &amp;0.055 &amp; &amp;0.498 &amp;0.250 &amp;0.332\\</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>167</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.88600000000000001</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.83599999999999997</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0.192</v>
+      </c>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="L10" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="M10" s="1">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1">
+        <v>0.46300000000000002</v>
+      </c>
+      <c r="P10" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="S10" t="str">
+        <f t="shared" si="0"/>
+        <v>PHM C01 SS - Low noise &amp;0.886 &amp;0.800 &amp;0.836 &amp;  &amp;0.380 &amp;0.130 &amp;0.192 &amp; &amp;0.400 &amp;0.020 &amp;0.038 &amp; &amp;0.463 &amp;0.140 &amp;0.207\\</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>168</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.78300000000000003</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.93</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.84899999999999998</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1">
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="L11" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="M11" s="1">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1">
+        <v>0.51900000000000002</v>
+      </c>
+      <c r="P11" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>0.28699999999999998</v>
+      </c>
+      <c r="S11" t="str">
+        <f t="shared" si="0"/>
+        <v>PHM C01 SS - High noise &amp;0.783 &amp;0.930 &amp;0.849 &amp;  &amp;0.000 &amp;0.000 &amp;0.000 &amp; &amp;0.508 &amp;0.960 &amp;0.664 &amp; &amp;0.519 &amp;0.210 &amp;0.287\\</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1">
+        <v>0.51300000000000001</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1">
+        <v>0.497</v>
+      </c>
+      <c r="L12" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="M12" s="1">
+        <v>0.65700000000000003</v>
+      </c>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="P12" s="1">
+        <v>0.47</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>0.47799999999999998</v>
+      </c>
+      <c r="S12" t="str">
+        <f t="shared" si="0"/>
+        <v>PHM C04 SS - No noise &amp;0.821 &amp;0.960 &amp;0.885 &amp;  &amp;0.513 &amp;0.090 &amp;0.149 &amp; &amp;0.497 &amp;0.970 &amp;0.657 &amp; &amp;0.489 &amp;0.470 &amp;0.478\\</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>169</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.73899999999999999</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1">
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0.51</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1">
+        <v>0.70599999999999996</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0.72</v>
+      </c>
+      <c r="M13" s="1">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1">
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="P13" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>0.36599999999999999</v>
+      </c>
+      <c r="S13" t="str">
+        <f t="shared" si="0"/>
+        <v>PHM C04 SS - Low noise &amp;0.739 &amp;0.990 &amp;0.846 &amp;  &amp;0.474 &amp;0.510 &amp;0.487 &amp; &amp;0.706 &amp;0.720 &amp;0.712 &amp; &amp;0.532 &amp;0.280 &amp;0.366\\</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>170</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.67100000000000004</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.78</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.72</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0.53400000000000003</v>
+      </c>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L14" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="M14" s="1">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="P14" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="S14" t="str">
+        <f t="shared" si="0"/>
+        <v>PHM C04 SS - High noise &amp;0.671 &amp;0.780 &amp;0.720 &amp;  &amp;0.522 &amp;0.550 &amp;0.534 &amp; &amp;0.500 &amp;0.980 &amp;0.662 &amp; &amp;0.472 &amp;0.250 &amp;0.325\\</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>160</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.78500000000000003</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0.46</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0.46100000000000002</v>
+      </c>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1">
+        <v>0.51100000000000001</v>
+      </c>
+      <c r="L15" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="M15" s="1">
+        <v>0.67100000000000004</v>
+      </c>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1">
+        <v>0.379</v>
+      </c>
+      <c r="P15" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="S15" t="str">
+        <f t="shared" si="0"/>
+        <v>PHM C06 SS - No noise &amp;1.000 &amp;0.650 &amp;0.785 &amp;  &amp;0.465 &amp;0.460 &amp;0.461 &amp; &amp;0.511 &amp;0.980 &amp;0.671 &amp; &amp;0.379 &amp;0.140 &amp;0.198\\</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>171</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.90200000000000002</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1">
+        <v>0.95099999999999996</v>
+      </c>
+      <c r="L16" s="1">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="M16" s="1">
+        <v>0.72</v>
+      </c>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="P16" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>0.432</v>
+      </c>
+      <c r="S16" t="str">
+        <f t="shared" si="0"/>
+        <v>PHM C06 SS - Low noise &amp;0.978 &amp;0.840 &amp;0.902 &amp;  &amp;0.493 &amp;0.530 &amp;0.508 &amp; &amp;0.951 &amp;0.580 &amp;0.720 &amp; &amp;0.500 &amp;0.380 &amp;0.432\\</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>172</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.78900000000000003</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1">
+        <v>0.505</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0.47</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0.48199999999999998</v>
+      </c>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1">
+        <v>0.505</v>
+      </c>
+      <c r="L17" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="M17" s="1">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1">
+        <v>0.36899999999999999</v>
+      </c>
+      <c r="P17" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="S17" t="str">
+        <f t="shared" si="0"/>
+        <v>PHM C06 SS - High noise &amp;0.715 &amp;0.880 &amp;0.789 &amp;  &amp;0.505 &amp;0.470 &amp;0.482 &amp; &amp;0.505 &amp;0.980 &amp;0.667 &amp; &amp;0.369 &amp;0.110 &amp;0.169\\</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>161</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.92</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0.59</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1">
+        <v>0.58399999999999996</v>
+      </c>
+      <c r="L18" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="M18" s="1">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="P18" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>0.313</v>
+      </c>
+      <c r="S18" t="str">
+        <f t="shared" si="0"/>
+        <v>PHM C01 MS - No noise &amp;0.798 &amp;0.920 &amp;0.852 &amp;  &amp;0.514 &amp;0.590 &amp;0.549 &amp; &amp;0.584 &amp;0.970 &amp;0.729 &amp; &amp;0.486 &amp;0.240 &amp;0.313\\</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>162</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0.69</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1">
+        <v>0.47599999999999998</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="L19" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="M19" s="1">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1">
+        <v>0.495</v>
+      </c>
+      <c r="P19" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>0.40100000000000002</v>
+      </c>
+      <c r="S19" t="str">
+        <f t="shared" si="0"/>
+        <v>PHM C04 MS - No noise &amp;0.774 &amp;0.690 &amp;0.728 &amp;  &amp;0.476 &amp;0.530 &amp;0.500 &amp; &amp;0.506 &amp;0.970 &amp;0.664 &amp; &amp;0.495 &amp;0.340 &amp;0.401\\</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>163</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="M20" s="1">
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1">
+        <v>0.44600000000000001</v>
+      </c>
+      <c r="P20" s="1">
+        <v>0.48</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>0.46</v>
+      </c>
+      <c r="S20" t="str">
+        <f t="shared" si="0"/>
+        <v>PHM C06 MS - No noise &amp;1.000 &amp;0.570 &amp;0.725 &amp;  &amp;0.491 &amp;0.600 &amp;0.536 &amp; &amp;0.492 &amp;0.960 &amp;0.651 &amp; &amp;0.446 &amp;0.480 &amp;0.460\\</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+      <c r="B23" s="75" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+      <c r="B24" s="75"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>175</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+      <c r="E25">
+        <v>4</v>
+      </c>
+      <c r="F25">
+        <v>5</v>
+      </c>
+      <c r="G25">
+        <v>6</v>
+      </c>
+      <c r="H25">
+        <v>7</v>
+      </c>
+      <c r="I25">
+        <v>8</v>
+      </c>
+      <c r="J25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B26" s="5"/>
+      <c r="C26" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26" s="5"/>
+      <c r="F26" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G26" s="5"/>
+      <c r="I26" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="J26" s="5"/>
+      <c r="L26" t="str">
+        <f>_xlfn.CONCAT(B26, " &amp;", C26, " &amp;", D26, " &amp;", E26, " &amp;", F26, " &amp;", G26, " &amp;", H26, " &amp;", I26, " &amp;", J26, " \\")</f>
+        <v xml:space="preserve"> &amp;Precision &amp; &amp; &amp;Recall &amp; &amp; &amp;F1-score &amp; \\</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="C27" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="L27" t="str">
+        <f>_xlfn.CONCAT(B27, " &amp;", C27, " &amp;", D27, " &amp;", E27, " &amp;", F27, " &amp;", G27, " &amp;", H27, " &amp;", I27, " &amp;", J27, " \\")</f>
+        <v xml:space="preserve"> &amp;Mean &amp;SD &amp; &amp;Mean &amp;SD &amp; &amp;Mean &amp;SD \\</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0.42867705419544677</v>
+      </c>
+      <c r="D28" s="3">
+        <v>8.7531082407871122E-2</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1">
+        <v>0.41113725490196051</v>
+      </c>
+      <c r="G28" s="3">
+        <v>8.5377782913454964E-2</v>
+      </c>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3">
+        <v>0.40295044267970159</v>
+      </c>
+      <c r="J28" s="1">
+        <v>6.9888457830582507E-2</v>
+      </c>
+      <c r="L28" t="str">
+        <f>_xlfn.CONCAT(B28, " &amp;", TEXT(C28, "0.000"), " &amp;", TEXT(D28, "0.000"), " &amp; &amp;",TEXT( F28,  "0.000"), " &amp;", TEXT(G28,  "0.000"), " &amp; &amp;", TEXT(I28,  "0.000"), " &amp;", TEXT(J28,  "0.000"), " \\")</f>
+        <v>A2C &amp;0.429 &amp;0.088 &amp; &amp;0.411 &amp;0.085 &amp; &amp;0.403 &amp;0.070 \\</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0.52911107506627419</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0.12067194028230305</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1">
+        <v>0.69262745098039225</v>
+      </c>
+      <c r="G29" s="3">
+        <v>3.4964787208832351E-2</v>
+      </c>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3">
+        <v>0.52090689324726325</v>
+      </c>
+      <c r="J29" s="1">
+        <v>2.805981213734909E-2</v>
+      </c>
+      <c r="L29" t="str">
+        <f>_xlfn.CONCAT(B29, " &amp;", TEXT(C29, "0.000"), " &amp;", TEXT(D29, "0.000"), " &amp; &amp;",TEXT( F29,  "0.000"), " &amp;", TEXT(G29,  "0.000"), " &amp; &amp;", TEXT(I29,  "0.000"), " &amp;", TEXT(J29,  "0.000"), " \\")</f>
+        <v>DQN &amp;0.529 &amp;0.121 &amp; &amp;0.693 &amp;0.035 &amp; &amp;0.521 &amp;0.028 \\</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0.47711924804775518</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0.15319259899601673</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1">
+        <v>0.26541176470588207</v>
+      </c>
+      <c r="G30" s="3">
+        <v>8.9551591423027307E-2</v>
+      </c>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3">
+        <v>0.31990474837618449</v>
+      </c>
+      <c r="J30" s="1">
+        <v>0.10129818207014342</v>
+      </c>
+      <c r="L30" t="str">
+        <f>_xlfn.CONCAT(B30, " &amp;", TEXT(C30, "0.000"), " &amp;", TEXT(D30, "0.000"), " &amp; &amp;",TEXT( F30,  "0.000"), " &amp;", TEXT(G30,  "0.000"), " &amp; &amp;", TEXT(I30,  "0.000"), " &amp;", TEXT(J30,  "0.000"), " \\")</f>
+        <v>PPO &amp;0.477 &amp;0.153 &amp; &amp;0.265 &amp;0.090 &amp; &amp;0.320 &amp;0.101 \\</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B31" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0.86870732223005609</v>
+      </c>
+      <c r="D31" s="3">
+        <v>3.8524356690436232E-2</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1">
+        <v>0.84752941176470575</v>
+      </c>
+      <c r="G31" s="3">
+        <v>6.1915357954097625E-2</v>
+      </c>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3">
+        <v>0.84200888071204683</v>
+      </c>
+      <c r="J31" s="1">
+        <v>4.4745355112257877E-2</v>
+      </c>
+      <c r="L31" t="str">
+        <f>_xlfn.CONCAT(B31, " &amp;", TEXT(C31, "0.000"), " &amp;", TEXT(D31, "0.000"), " &amp; &amp;",TEXT( F31,  "0.000"), " &amp;", TEXT(G31,  "0.000"), " &amp; &amp;", TEXT(I31,  "0.000"), " &amp;", TEXT(J31,  "0.000"), " \\")</f>
+        <v>REINFORCE &amp;0.869 &amp;0.039 &amp; &amp;0.848 &amp;0.062 &amp; &amp;0.842 &amp;0.045 \\</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <v>3</v>
+      </c>
+      <c r="E33">
+        <v>4</v>
+      </c>
+      <c r="F33">
+        <v>5</v>
+      </c>
+      <c r="G33">
+        <v>6</v>
+      </c>
+      <c r="H33">
+        <v>7</v>
+      </c>
+      <c r="I33">
+        <v>8</v>
+      </c>
+      <c r="J33">
+        <v>9</v>
+      </c>
+      <c r="K33">
+        <v>10</v>
+      </c>
+      <c r="L33">
+        <v>11</v>
+      </c>
+      <c r="M33">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B34" s="68" t="s">
+        <v>176</v>
+      </c>
+      <c r="C34" s="68" t="s">
+        <v>177</v>
+      </c>
+      <c r="D34" s="68" t="s">
+        <v>178</v>
+      </c>
+      <c r="E34" s="68" t="s">
+        <v>179</v>
+      </c>
+      <c r="F34" s="68" t="s">
+        <v>180</v>
+      </c>
+      <c r="G34" s="68" t="s">
+        <v>181</v>
+      </c>
+      <c r="H34" s="68" t="s">
+        <v>182</v>
+      </c>
+      <c r="I34" s="68" t="s">
+        <v>183</v>
+      </c>
+      <c r="J34" s="68" t="s">
+        <v>184</v>
+      </c>
+      <c r="K34" s="68" t="s">
+        <v>185</v>
+      </c>
+      <c r="L34" s="68" t="s">
+        <v>186</v>
+      </c>
+      <c r="M34" s="68" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B35" s="5"/>
+      <c r="C35" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D35" s="5"/>
+      <c r="F35" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G35" s="5"/>
+      <c r="I35" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="J35" s="5"/>
+      <c r="L35" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="M35" s="5"/>
+      <c r="O35" t="str">
+        <f>_xlfn.CONCAT(B35, " &amp;", C35, " &amp;", D35, " &amp;", E35, " &amp;", F35, " &amp;", G35, " &amp;", H35, " &amp;", I35, " &amp;", J35,   "&amp;", K35, " &amp;", L35,  " \\")</f>
+        <v xml:space="preserve"> &amp;Precision &amp; &amp; &amp;Recall &amp; &amp; &amp;F1-score &amp;&amp; &amp;F-beta score (0.5) \\</v>
+      </c>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C36" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J36" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="L36" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="M36" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="O36" t="str">
+        <f>_xlfn.CONCAT(B36, " &amp;", C36, " &amp;", D36, " &amp;", E36, " &amp;", F36, " &amp;", G36, " &amp;", H36, " &amp;", I36, " &amp;", J36,   "&amp;", K36, " &amp;", L36,  " \\")</f>
+        <v xml:space="preserve"> &amp;Mean &amp;SD &amp; &amp;Mean &amp;SD &amp; &amp;Mean &amp;SD&amp; &amp;Mean \\</v>
+      </c>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" s="3">
+        <v>1</v>
+      </c>
+      <c r="D37" s="3">
+        <v>2</v>
+      </c>
+      <c r="F37" s="3">
+        <v>3</v>
+      </c>
+      <c r="G37" s="3">
+        <v>4</v>
+      </c>
+      <c r="I37" s="3">
+        <v>5</v>
+      </c>
+      <c r="J37" s="3">
+        <v>6</v>
+      </c>
+      <c r="L37" s="3">
+        <v>7</v>
+      </c>
+      <c r="M37" s="3">
+        <v>8</v>
+      </c>
+      <c r="O37" t="str">
+        <f>_xlfn.CONCAT(B37, " &amp;", TEXT(C37, "0.000"), " &amp;", TEXT(D37, "0.000"), " &amp;  &amp;",  ,TEXT( F37,  "0.000"), " &amp;", TEXT(G37,  "0.000"), " &amp; &amp; ",  TEXT(I37,  "0.000"), " &amp;", TEXT(J37,  "0.000"), " &amp; &amp;", TEXT(L37,  "0.000"), " &amp;", TEXT(M37,  "0.000"), " \\")</f>
+        <v>A2C &amp;1.000 &amp;2.000 &amp;  &amp;3.000 &amp;4.000 &amp; &amp; 5.000 &amp;6.000 &amp; &amp;7.000 &amp;8.000 \\</v>
+      </c>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" s="3">
+        <v>1</v>
+      </c>
+      <c r="D38" s="3">
+        <v>2</v>
+      </c>
+      <c r="F38" s="3">
+        <v>3</v>
+      </c>
+      <c r="G38" s="3">
+        <v>4</v>
+      </c>
+      <c r="I38" s="3">
+        <v>5</v>
+      </c>
+      <c r="J38" s="3">
+        <v>6</v>
+      </c>
+      <c r="L38" s="3">
+        <v>7</v>
+      </c>
+      <c r="M38" s="3">
+        <v>8</v>
+      </c>
+      <c r="O38" t="str">
+        <f t="shared" ref="O38:O40" si="1">_xlfn.CONCAT(B38, " &amp;", TEXT(C38, "0.000"), " &amp;", TEXT(D38, "0.000"), " &amp;  &amp;",  ,TEXT( F38,  "0.000"), " &amp;", TEXT(G38,  "0.000"), " &amp; &amp; ",  TEXT(I38,  "0.000"), " &amp;", TEXT(J38,  "0.000"), " &amp; &amp;", TEXT(L38,  "0.000"), " &amp;", TEXT(M38,  "0.000"), " \\")</f>
+        <v>DQN &amp;1.000 &amp;2.000 &amp;  &amp;3.000 &amp;4.000 &amp; &amp; 5.000 &amp;6.000 &amp; &amp;7.000 &amp;8.000 \\</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39" s="3">
+        <v>1</v>
+      </c>
+      <c r="D39" s="3">
+        <v>2</v>
+      </c>
+      <c r="F39" s="3">
+        <v>3</v>
+      </c>
+      <c r="G39" s="3">
+        <v>4</v>
+      </c>
+      <c r="I39" s="3">
+        <v>5</v>
+      </c>
+      <c r="J39" s="3">
+        <v>6</v>
+      </c>
+      <c r="L39" s="3">
+        <v>7</v>
+      </c>
+      <c r="M39" s="3">
+        <v>8</v>
+      </c>
+      <c r="O39" t="str">
+        <f t="shared" si="1"/>
+        <v>PPO &amp;1.000 &amp;2.000 &amp;  &amp;3.000 &amp;4.000 &amp; &amp; 5.000 &amp;6.000 &amp; &amp;7.000 &amp;8.000 \\</v>
+      </c>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B40" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C40" s="3">
+        <v>1</v>
+      </c>
+      <c r="D40" s="3">
+        <v>2</v>
+      </c>
+      <c r="F40" s="3">
+        <v>3</v>
+      </c>
+      <c r="G40" s="3">
+        <v>4</v>
+      </c>
+      <c r="I40" s="3">
+        <v>5</v>
+      </c>
+      <c r="J40" s="3">
+        <v>6</v>
+      </c>
+      <c r="L40" s="3">
+        <v>7</v>
+      </c>
+      <c r="M40" s="3">
+        <v>8</v>
+      </c>
+      <c r="O40" t="str">
+        <f t="shared" si="1"/>
+        <v>REINFORCE &amp;1.000 &amp;2.000 &amp;  &amp;3.000 &amp;4.000 &amp; &amp; 5.000 &amp;6.000 &amp; &amp;7.000 &amp;8.000 \\</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F400A2A3-4CEA-47B2-96F4-E5BC0FCEB5FA}">
   <dimension ref="A1:AO50"/>
   <sheetViews>
@@ -4311,19 +5594,19 @@
       <selection pane="bottomLeft" activeCell="V38" sqref="V38:AB43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="38.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="43.5703125" hidden="1" customWidth="1"/>
-    <col min="7" max="10" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" hidden="1" customWidth="1"/>
-    <col min="12" max="13" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="24.140625" customWidth="1"/>
-    <col min="17" max="17" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="43.5546875" hidden="1" customWidth="1"/>
+    <col min="7" max="10" width="9.109375" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" hidden="1" customWidth="1"/>
+    <col min="12" max="13" width="9.109375" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="24.109375" customWidth="1"/>
+    <col min="17" max="17" width="8.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4439,7 +5722,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -4558,7 +5841,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4677,7 +5960,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:39" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:39" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -4796,7 +6079,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:39" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -4912,7 +6195,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -5028,7 +6311,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -5144,7 +6427,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -5260,7 +6543,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -5376,7 +6659,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -5492,7 +6775,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -5608,7 +6891,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -5724,7 +7007,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:39" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:39" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -5840,7 +7123,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:39" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:39" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -5956,7 +7239,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -6072,7 +7355,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:39" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:39" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -6188,8 +7471,8 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="4:41" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="4:41" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:41" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="4:41" x14ac:dyDescent="0.3">
       <c r="N18" t="s">
         <v>107</v>
       </c>
@@ -6244,9 +7527,9 @@
       <c r="AM18" s="1"/>
       <c r="AO18" s="1"/>
     </row>
-    <row r="20" spans="4:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="4:41" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="4:41" ht="21" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="4:41" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="4:41" ht="21" x14ac:dyDescent="0.4">
       <c r="D23" s="10" t="s">
         <v>108</v>
       </c>
@@ -6351,8 +7634,8 @@
       </c>
       <c r="AM23" s="2"/>
     </row>
-    <row r="24" spans="4:41" x14ac:dyDescent="0.25">
-      <c r="D24" s="76" t="s">
+    <row r="24" spans="4:41" x14ac:dyDescent="0.3">
+      <c r="D24" s="77" t="s">
         <v>104</v>
       </c>
       <c r="N24" t="s">
@@ -6456,8 +7739,8 @@
       </c>
       <c r="AM24" s="2"/>
     </row>
-    <row r="25" spans="4:41" x14ac:dyDescent="0.25">
-      <c r="D25" s="76"/>
+    <row r="25" spans="4:41" x14ac:dyDescent="0.3">
+      <c r="D25" s="77"/>
       <c r="N25" t="s">
         <v>70</v>
       </c>
@@ -6559,8 +7842,8 @@
       </c>
       <c r="AM25" s="2"/>
     </row>
-    <row r="26" spans="4:41" x14ac:dyDescent="0.25">
-      <c r="D26" s="76"/>
+    <row r="26" spans="4:41" x14ac:dyDescent="0.3">
+      <c r="D26" s="77"/>
       <c r="N26" s="5" t="s">
         <v>68</v>
       </c>
@@ -6662,7 +7945,7 @@
       </c>
       <c r="AM26" s="2"/>
     </row>
-    <row r="28" spans="4:41" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:41" x14ac:dyDescent="0.3">
       <c r="N28" s="5" t="s">
         <v>72</v>
       </c>
@@ -6670,35 +7953,35 @@
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="4:41" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:41" x14ac:dyDescent="0.3">
       <c r="N29" s="5"/>
-      <c r="O29" s="77" t="s">
+      <c r="O29" s="76" t="s">
         <v>79</v>
       </c>
-      <c r="P29" s="77"/>
-      <c r="Q29" s="77" t="s">
+      <c r="P29" s="76"/>
+      <c r="Q29" s="76" t="s">
         <v>82</v>
       </c>
-      <c r="R29" s="77"/>
-      <c r="S29" s="77" t="s">
+      <c r="R29" s="76"/>
+      <c r="S29" s="76" t="s">
         <v>83</v>
       </c>
-      <c r="T29" s="77"/>
+      <c r="T29" s="76"/>
       <c r="V29" s="5"/>
-      <c r="W29" s="77" t="s">
+      <c r="W29" s="76" t="s">
         <v>79</v>
       </c>
-      <c r="X29" s="77"/>
-      <c r="Y29" s="77" t="s">
+      <c r="X29" s="76"/>
+      <c r="Y29" s="76" t="s">
         <v>82</v>
       </c>
-      <c r="Z29" s="77"/>
-      <c r="AA29" s="77" t="s">
+      <c r="Z29" s="76"/>
+      <c r="AA29" s="76" t="s">
         <v>83</v>
       </c>
-      <c r="AB29" s="77"/>
-    </row>
-    <row r="30" spans="4:41" x14ac:dyDescent="0.25">
+      <c r="AB29" s="76"/>
+    </row>
+    <row r="30" spans="4:41" x14ac:dyDescent="0.3">
       <c r="O30" s="6" t="s">
         <v>80</v>
       </c>
@@ -6736,7 +8019,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="4:41" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:41" x14ac:dyDescent="0.3">
       <c r="N31" t="s">
         <v>63</v>
       </c>
@@ -6792,7 +8075,7 @@
         <v>9.2300000000000007E-2</v>
       </c>
     </row>
-    <row r="32" spans="4:41" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:41" x14ac:dyDescent="0.3">
       <c r="N32" t="s">
         <v>64</v>
       </c>
@@ -6848,7 +8131,7 @@
         <v>3.15E-2</v>
       </c>
     </row>
-    <row r="33" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="33" spans="14:28" x14ac:dyDescent="0.3">
       <c r="N33" t="s">
         <v>65</v>
       </c>
@@ -6904,7 +8187,7 @@
         <v>8.826666666666666E-2</v>
       </c>
     </row>
-    <row r="34" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="34" spans="14:28" x14ac:dyDescent="0.3">
       <c r="N34" s="12" t="s">
         <v>66</v>
       </c>
@@ -6960,7 +8243,7 @@
         <v>2.5033333333333335E-2</v>
       </c>
     </row>
-    <row r="35" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="35" spans="14:28" x14ac:dyDescent="0.3">
       <c r="O35" s="1">
         <f>O34-MAX(O31:O33)</f>
         <v>0.36503125000000003</v>
@@ -7010,7 +8293,7 @@
         <v>-3.6558222222222222E-4</v>
       </c>
     </row>
-    <row r="37" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="37" spans="14:28" x14ac:dyDescent="0.3">
       <c r="N37" s="5" t="s">
         <v>73</v>
       </c>
@@ -7018,35 +8301,35 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="38" spans="14:28" x14ac:dyDescent="0.3">
       <c r="N38" s="5"/>
-      <c r="O38" s="77" t="s">
+      <c r="O38" s="76" t="s">
         <v>79</v>
       </c>
-      <c r="P38" s="77"/>
-      <c r="Q38" s="77" t="s">
+      <c r="P38" s="76"/>
+      <c r="Q38" s="76" t="s">
         <v>82</v>
       </c>
-      <c r="R38" s="77"/>
-      <c r="S38" s="77" t="s">
+      <c r="R38" s="76"/>
+      <c r="S38" s="76" t="s">
         <v>83</v>
       </c>
-      <c r="T38" s="77"/>
+      <c r="T38" s="76"/>
       <c r="V38" s="5"/>
-      <c r="W38" s="77" t="s">
+      <c r="W38" s="76" t="s">
         <v>79</v>
       </c>
-      <c r="X38" s="77"/>
-      <c r="Y38" s="77" t="s">
+      <c r="X38" s="76"/>
+      <c r="Y38" s="76" t="s">
         <v>82</v>
       </c>
-      <c r="Z38" s="77"/>
-      <c r="AA38" s="77" t="s">
+      <c r="Z38" s="76"/>
+      <c r="AA38" s="76" t="s">
         <v>83</v>
       </c>
-      <c r="AB38" s="77"/>
-    </row>
-    <row r="39" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="AB38" s="76"/>
+    </row>
+    <row r="39" spans="14:28" x14ac:dyDescent="0.3">
       <c r="O39" s="6" t="s">
         <v>80</v>
       </c>
@@ -7084,7 +8367,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="40" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="40" spans="14:28" x14ac:dyDescent="0.3">
       <c r="N40" t="s">
         <v>63</v>
       </c>
@@ -7140,7 +8423,7 @@
         <v>5.9633333333333337E-2</v>
       </c>
     </row>
-    <row r="41" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="41" spans="14:28" x14ac:dyDescent="0.3">
       <c r="N41" t="s">
         <v>64</v>
       </c>
@@ -7196,7 +8479,7 @@
         <v>7.273333333333333E-2</v>
       </c>
     </row>
-    <row r="42" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="42" spans="14:28" x14ac:dyDescent="0.3">
       <c r="N42" t="s">
         <v>65</v>
       </c>
@@ -7252,7 +8535,7 @@
         <v>8.0133333333333334E-2</v>
       </c>
     </row>
-    <row r="43" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="43" spans="14:28" x14ac:dyDescent="0.3">
       <c r="N43" s="12" t="s">
         <v>66</v>
       </c>
@@ -7308,7 +8591,7 @@
         <v>4.5233333333333327E-2</v>
       </c>
     </row>
-    <row r="44" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="44" spans="14:28" x14ac:dyDescent="0.3">
       <c r="O44" s="1">
         <f>O43-MAX(O40:O42)</f>
         <v>0.33702222222222222</v>
@@ -7358,10 +8641,10 @@
         <v>-1.5100800000000009E-3</v>
       </c>
     </row>
-    <row r="45" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="45" spans="14:28" x14ac:dyDescent="0.3">
       <c r="O45" s="1"/>
     </row>
-    <row r="46" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="46" spans="14:28" x14ac:dyDescent="0.3">
       <c r="N46" t="s">
         <v>84</v>
       </c>
@@ -7373,7 +8656,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="47" spans="14:28" x14ac:dyDescent="0.3">
       <c r="Q47" s="1">
         <f>AVERAGE(P35,R35,T35,X35,Z35,AB35,P44,R44,T44,X44,Z44,AB44)</f>
         <v>-7.1771071069958879E-4</v>
@@ -7382,10 +8665,10 @@
         <v>102</v>
       </c>
     </row>
-    <row r="48" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="48" spans="14:28" x14ac:dyDescent="0.3">
       <c r="Q48" s="8"/>
     </row>
-    <row r="49" spans="14:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="14:17" x14ac:dyDescent="0.3">
       <c r="N49" t="s">
         <v>103</v>
       </c>
@@ -7394,7 +8677,7 @@
         <v>0.36597170138888885</v>
       </c>
     </row>
-    <row r="50" spans="14:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="14:17" x14ac:dyDescent="0.3">
       <c r="Q50" s="1">
         <f>AVERAGE(P35,X35,P44,X44)</f>
         <v>-3.3208198123456799E-3</v>
@@ -7402,6 +8685,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="S29:T29"/>
+    <mergeCell ref="W29:X29"/>
     <mergeCell ref="AA29:AB29"/>
     <mergeCell ref="O38:P38"/>
     <mergeCell ref="Q38:R38"/>
@@ -7410,11 +8698,6 @@
     <mergeCell ref="Y38:Z38"/>
     <mergeCell ref="AA38:AB38"/>
     <mergeCell ref="Y29:Z29"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="Q29:R29"/>
-    <mergeCell ref="S29:T29"/>
-    <mergeCell ref="W29:X29"/>
   </mergeCells>
   <conditionalFormatting sqref="W2:W16">
     <cfRule type="cellIs" dxfId="95" priority="12" operator="greaterThan">
@@ -7504,7 +8787,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2CE5ED4-D8F3-4069-9277-95EE791A9F93}">
   <dimension ref="A1:AO50"/>
   <sheetViews>
@@ -7513,19 +8796,19 @@
       <selection pane="bottomLeft" activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="38.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="43.5703125" hidden="1" customWidth="1"/>
-    <col min="7" max="10" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" hidden="1" customWidth="1"/>
-    <col min="12" max="13" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="24.140625" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="43.5546875" hidden="1" customWidth="1"/>
+    <col min="7" max="10" width="9.109375" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" hidden="1" customWidth="1"/>
+    <col min="12" max="13" width="9.109375" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="24.109375" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="8.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
@@ -7641,7 +8924,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -7760,7 +9043,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -7879,7 +9162,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:39" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:39" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -7998,7 +9281,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:39" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -8114,7 +9397,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -8230,7 +9513,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -8346,7 +9629,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -8462,7 +9745,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -8578,7 +9861,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -8694,7 +9977,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -8810,7 +10093,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -8926,7 +10209,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:39" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:39" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -9042,7 +10325,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:39" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:39" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -9158,7 +10441,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -9274,7 +10557,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:39" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:39" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -9390,8 +10673,8 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="4:41" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="4:41" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:41" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="4:41" x14ac:dyDescent="0.3">
       <c r="N18" t="s">
         <v>107</v>
       </c>
@@ -9446,9 +10729,9 @@
       <c r="AM18" s="1"/>
       <c r="AO18" s="1"/>
     </row>
-    <row r="20" spans="4:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="4:41" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="4:41" ht="21" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="4:41" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="4:41" ht="21" x14ac:dyDescent="0.4">
       <c r="D23" s="10" t="s">
         <v>106</v>
       </c>
@@ -9553,8 +10836,8 @@
       </c>
       <c r="AM23" s="2"/>
     </row>
-    <row r="24" spans="4:41" x14ac:dyDescent="0.25">
-      <c r="D24" s="76" t="s">
+    <row r="24" spans="4:41" x14ac:dyDescent="0.3">
+      <c r="D24" s="77" t="s">
         <v>104</v>
       </c>
       <c r="N24" t="s">
@@ -9658,8 +10941,8 @@
       </c>
       <c r="AM24" s="2"/>
     </row>
-    <row r="25" spans="4:41" x14ac:dyDescent="0.25">
-      <c r="D25" s="76"/>
+    <row r="25" spans="4:41" x14ac:dyDescent="0.3">
+      <c r="D25" s="77"/>
       <c r="N25" t="s">
         <v>70</v>
       </c>
@@ -9761,8 +11044,8 @@
       </c>
       <c r="AM25" s="2"/>
     </row>
-    <row r="26" spans="4:41" x14ac:dyDescent="0.25">
-      <c r="D26" s="76"/>
+    <row r="26" spans="4:41" x14ac:dyDescent="0.3">
+      <c r="D26" s="77"/>
       <c r="N26" s="5" t="s">
         <v>68</v>
       </c>
@@ -9864,7 +11147,7 @@
       </c>
       <c r="AM26" s="2"/>
     </row>
-    <row r="28" spans="4:41" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:41" x14ac:dyDescent="0.3">
       <c r="N28" s="5" t="s">
         <v>72</v>
       </c>
@@ -9872,35 +11155,35 @@
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="4:41" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:41" x14ac:dyDescent="0.3">
       <c r="N29" s="5"/>
-      <c r="O29" s="77" t="s">
+      <c r="O29" s="76" t="s">
         <v>79</v>
       </c>
-      <c r="P29" s="77"/>
-      <c r="Q29" s="77" t="s">
+      <c r="P29" s="76"/>
+      <c r="Q29" s="76" t="s">
         <v>82</v>
       </c>
-      <c r="R29" s="77"/>
-      <c r="S29" s="77" t="s">
+      <c r="R29" s="76"/>
+      <c r="S29" s="76" t="s">
         <v>83</v>
       </c>
-      <c r="T29" s="77"/>
+      <c r="T29" s="76"/>
       <c r="V29" s="5"/>
-      <c r="W29" s="77" t="s">
+      <c r="W29" s="76" t="s">
         <v>79</v>
       </c>
-      <c r="X29" s="77"/>
-      <c r="Y29" s="77" t="s">
+      <c r="X29" s="76"/>
+      <c r="Y29" s="76" t="s">
         <v>82</v>
       </c>
-      <c r="Z29" s="77"/>
-      <c r="AA29" s="77" t="s">
+      <c r="Z29" s="76"/>
+      <c r="AA29" s="76" t="s">
         <v>83</v>
       </c>
-      <c r="AB29" s="77"/>
-    </row>
-    <row r="30" spans="4:41" x14ac:dyDescent="0.25">
+      <c r="AB29" s="76"/>
+    </row>
+    <row r="30" spans="4:41" x14ac:dyDescent="0.3">
       <c r="O30" s="6" t="s">
         <v>80</v>
       </c>
@@ -9938,7 +11221,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="4:41" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:41" x14ac:dyDescent="0.3">
       <c r="N31" t="s">
         <v>63</v>
       </c>
@@ -9994,7 +11277,7 @@
         <v>8.666666666666667E-2</v>
       </c>
     </row>
-    <row r="32" spans="4:41" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:41" x14ac:dyDescent="0.3">
       <c r="N32" t="s">
         <v>64</v>
       </c>
@@ -10050,7 +11333,7 @@
         <v>1.6666666666666666E-2</v>
       </c>
     </row>
-    <row r="33" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="33" spans="14:28" x14ac:dyDescent="0.3">
       <c r="N33" t="s">
         <v>65</v>
       </c>
@@ -10106,7 +11389,7 @@
         <v>6.3333333333333339E-2</v>
       </c>
     </row>
-    <row r="34" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="34" spans="14:28" x14ac:dyDescent="0.3">
       <c r="N34" s="12" t="s">
         <v>66</v>
       </c>
@@ -10162,7 +11445,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="35" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="35" spans="14:28" x14ac:dyDescent="0.3">
       <c r="O35" s="1">
         <f>O34-MAX(O31:O33)</f>
         <v>0.39750000000000002</v>
@@ -10212,7 +11495,7 @@
         <v>1.3222222222222222E-3</v>
       </c>
     </row>
-    <row r="37" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="37" spans="14:28" x14ac:dyDescent="0.3">
       <c r="N37" s="5" t="s">
         <v>73</v>
       </c>
@@ -10220,35 +11503,35 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="38" spans="14:28" x14ac:dyDescent="0.3">
       <c r="N38" s="5"/>
-      <c r="O38" s="77" t="s">
+      <c r="O38" s="76" t="s">
         <v>79</v>
       </c>
-      <c r="P38" s="77"/>
-      <c r="Q38" s="77" t="s">
+      <c r="P38" s="76"/>
+      <c r="Q38" s="76" t="s">
         <v>82</v>
       </c>
-      <c r="R38" s="77"/>
-      <c r="S38" s="77" t="s">
+      <c r="R38" s="76"/>
+      <c r="S38" s="76" t="s">
         <v>83</v>
       </c>
-      <c r="T38" s="77"/>
+      <c r="T38" s="76"/>
       <c r="V38" s="5"/>
-      <c r="W38" s="77" t="s">
+      <c r="W38" s="76" t="s">
         <v>79</v>
       </c>
-      <c r="X38" s="77"/>
-      <c r="Y38" s="77" t="s">
+      <c r="X38" s="76"/>
+      <c r="Y38" s="76" t="s">
         <v>82</v>
       </c>
-      <c r="Z38" s="77"/>
-      <c r="AA38" s="77" t="s">
+      <c r="Z38" s="76"/>
+      <c r="AA38" s="76" t="s">
         <v>83</v>
       </c>
-      <c r="AB38" s="77"/>
-    </row>
-    <row r="39" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="AB38" s="76"/>
+    </row>
+    <row r="39" spans="14:28" x14ac:dyDescent="0.3">
       <c r="O39" s="6" t="s">
         <v>80</v>
       </c>
@@ -10286,7 +11569,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="40" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="40" spans="14:28" x14ac:dyDescent="0.3">
       <c r="N40" t="s">
         <v>63</v>
       </c>
@@ -10342,7 +11625,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="41" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="41" spans="14:28" x14ac:dyDescent="0.3">
       <c r="N41" t="s">
         <v>64</v>
       </c>
@@ -10398,7 +11681,7 @@
         <v>5.3333333333333344E-2</v>
       </c>
     </row>
-    <row r="42" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="42" spans="14:28" x14ac:dyDescent="0.3">
       <c r="N42" t="s">
         <v>65</v>
       </c>
@@ -10454,7 +11737,7 @@
         <v>9.6666666666666665E-2</v>
       </c>
     </row>
-    <row r="43" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="43" spans="14:28" x14ac:dyDescent="0.3">
       <c r="N43" s="12" t="s">
         <v>66</v>
       </c>
@@ -10510,7 +11793,7 @@
         <v>5.6666666666666671E-2</v>
       </c>
     </row>
-    <row r="44" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="44" spans="14:28" x14ac:dyDescent="0.3">
       <c r="O44" s="1">
         <f>O43-MAX(O40:O42)</f>
         <v>0.3677777777777777</v>
@@ -10560,10 +11843,10 @@
         <v>1.6111111111111116E-3</v>
       </c>
     </row>
-    <row r="45" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="45" spans="14:28" x14ac:dyDescent="0.3">
       <c r="O45" s="1"/>
     </row>
-    <row r="46" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="46" spans="14:28" x14ac:dyDescent="0.3">
       <c r="N46" t="s">
         <v>84</v>
       </c>
@@ -10575,7 +11858,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="47" spans="14:28" x14ac:dyDescent="0.3">
       <c r="Q47" s="1">
         <f>AVERAGE(P35,R35,T35,X35,Z35,AB35,P44,R44,T44,X44,Z44,AB44)</f>
         <v>1.3346913580246914E-4</v>
@@ -10584,10 +11867,10 @@
         <v>102</v>
       </c>
     </row>
-    <row r="48" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="48" spans="14:28" x14ac:dyDescent="0.3">
       <c r="Q48" s="8"/>
     </row>
-    <row r="49" spans="14:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="14:17" x14ac:dyDescent="0.3">
       <c r="N49" t="s">
         <v>103</v>
       </c>
@@ -10596,7 +11879,7 @@
         <v>0.38631944444444444</v>
       </c>
     </row>
-    <row r="50" spans="14:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="14:17" x14ac:dyDescent="0.3">
       <c r="Q50" s="1">
         <f>AVERAGE(P35,X35,P44,X44)</f>
         <v>-2.9198395061728406E-3</v>
@@ -10678,49 +11961,49 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18D2DBEF-0F10-45BF-A4F0-C0A5C8C71E73}">
   <dimension ref="A1:AX52"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AT5" sqref="AT5"/>
+      <selection pane="bottomLeft" activeCell="AT13" sqref="AT13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="43.5703125" style="14" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="43.5703125" hidden="1" customWidth="1"/>
-    <col min="7" max="10" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" hidden="1" customWidth="1"/>
-    <col min="12" max="13" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="24.140625" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="0.7109375" customWidth="1"/>
+    <col min="4" max="4" width="43.5546875" style="14" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="43.5546875" hidden="1" customWidth="1"/>
+    <col min="7" max="10" width="9.109375" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" hidden="1" customWidth="1"/>
+    <col min="12" max="13" width="9.109375" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="24.109375" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="0.6640625" customWidth="1"/>
     <col min="17" max="17" width="0" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="0" hidden="1" customWidth="1"/>
     <col min="21" max="21" width="0" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="0.7109375" customWidth="1"/>
+    <col min="22" max="22" width="0.6640625" customWidth="1"/>
     <col min="24" max="24" width="0" hidden="1" customWidth="1"/>
     <col min="26" max="26" width="0" hidden="1" customWidth="1"/>
     <col min="28" max="28" width="0" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="0.7109375" customWidth="1"/>
+    <col min="29" max="29" width="0.6640625" customWidth="1"/>
     <col min="31" max="31" width="0" hidden="1" customWidth="1"/>
     <col min="33" max="33" width="0" hidden="1" customWidth="1"/>
     <col min="35" max="35" width="0" hidden="1" customWidth="1"/>
-    <col min="36" max="36" width="0.7109375" customWidth="1"/>
+    <col min="36" max="36" width="0.6640625" customWidth="1"/>
     <col min="38" max="38" width="0" hidden="1" customWidth="1"/>
     <col min="40" max="40" width="0" hidden="1" customWidth="1"/>
     <col min="42" max="43" width="0" hidden="1" customWidth="1"/>
-    <col min="44" max="44" width="2.140625" customWidth="1"/>
-    <col min="45" max="45" width="4.85546875" customWidth="1"/>
-    <col min="46" max="46" width="9.85546875" customWidth="1"/>
+    <col min="44" max="44" width="2.109375" customWidth="1"/>
+    <col min="45" max="45" width="4.88671875" customWidth="1"/>
+    <col min="46" max="46" width="9.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" ht="4.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:50" x14ac:dyDescent="0.3">
       <c r="D2" s="48"/>
       <c r="E2" s="49"/>
       <c r="F2" s="49"/>
@@ -10764,7 +12047,7 @@
       <c r="AN2" s="82"/>
       <c r="AO2" s="83"/>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.3">
       <c r="D3" s="43"/>
       <c r="E3" s="26"/>
       <c r="F3" s="26"/>
@@ -10810,7 +12093,7 @@
       <c r="AN3" s="86"/>
       <c r="AO3" s="87"/>
     </row>
-    <row r="4" spans="1:50" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:50" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>0</v>
       </c>
@@ -10917,7 +12200,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:50" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:50" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0</v>
       </c>
@@ -11044,7 +12327,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:50" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:50" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -11171,7 +12454,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:50" s="16" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:50" s="16" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16">
         <v>2</v>
       </c>
@@ -11301,7 +12584,7 @@
       <c r="AW7"/>
       <c r="AX7"/>
     </row>
-    <row r="8" spans="1:50" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:50" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3</v>
       </c>
@@ -11422,7 +12705,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:50" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:50" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>4</v>
       </c>
@@ -11543,7 +12826,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:50" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:50" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>5</v>
       </c>
@@ -11664,7 +12947,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:50" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:50" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>6</v>
       </c>
@@ -11785,7 +13068,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:50" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:50" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>7</v>
       </c>
@@ -11906,7 +13189,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:50" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:50" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>8</v>
       </c>
@@ -12027,7 +13310,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:50" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:50" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>9</v>
       </c>
@@ -12148,7 +13431,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:50" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:50" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>10</v>
       </c>
@@ -12269,7 +13552,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:50" s="16" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:50" s="16" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16">
         <v>11</v>
       </c>
@@ -12397,7 +13680,7 @@
       <c r="AW16"/>
       <c r="AX16"/>
     </row>
-    <row r="17" spans="1:50" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:50" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>12</v>
       </c>
@@ -12518,7 +13801,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:50" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:50" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>13</v>
       </c>
@@ -12639,7 +13922,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:50" s="4" customFormat="1" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:50" s="4" customFormat="1" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
         <v>14</v>
       </c>
@@ -12767,7 +14050,7 @@
       <c r="AW19"/>
       <c r="AX19"/>
     </row>
-    <row r="20" spans="1:50" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:50" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="D20" s="47" t="s">
         <v>110</v>
       </c>
@@ -12849,7 +14132,7 @@
       <c r="AQ20" s="1"/>
       <c r="AS20" s="1"/>
     </row>
-    <row r="21" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:50" x14ac:dyDescent="0.3">
       <c r="D21" s="52" t="s">
         <v>111</v>
       </c>
@@ -12927,7 +14210,7 @@
         <v>0.32792536211839812</v>
       </c>
     </row>
-    <row r="22" spans="1:50" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:50" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D22" s="15"/>
       <c r="AR22"/>
       <c r="AS22"/>
@@ -12937,8 +14220,8 @@
       <c r="AW22"/>
       <c r="AX22"/>
     </row>
-    <row r="23" spans="1:50" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:50" ht="21" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:50" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:50" ht="21" x14ac:dyDescent="0.4">
       <c r="D25" s="24" t="s">
         <v>109</v>
       </c>
@@ -13046,7 +14329,7 @@
       </c>
       <c r="AQ25" s="2"/>
     </row>
-    <row r="26" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:50" x14ac:dyDescent="0.3">
       <c r="D26" s="84" t="s">
         <v>104</v>
       </c>
@@ -13154,7 +14437,7 @@
       </c>
       <c r="AQ26" s="2"/>
     </row>
-    <row r="27" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:50" x14ac:dyDescent="0.3">
       <c r="D27" s="84"/>
       <c r="N27" t="s">
         <v>70</v>
@@ -13260,7 +14543,7 @@
       </c>
       <c r="AQ27" s="2"/>
     </row>
-    <row r="28" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:50" x14ac:dyDescent="0.3">
       <c r="D28" s="84"/>
       <c r="N28" s="5" t="s">
         <v>68</v>
@@ -13367,7 +14650,7 @@
       </c>
       <c r="AQ28" s="2"/>
     </row>
-    <row r="30" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:50" x14ac:dyDescent="0.3">
       <c r="N30" s="5" t="s">
         <v>72</v>
       </c>
@@ -13376,38 +14659,38 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:50" x14ac:dyDescent="0.3">
       <c r="N31" s="5"/>
       <c r="O31" s="5"/>
-      <c r="P31" s="77" t="s">
+      <c r="P31" s="76" t="s">
         <v>79</v>
       </c>
-      <c r="Q31" s="77"/>
-      <c r="R31" s="77" t="s">
+      <c r="Q31" s="76"/>
+      <c r="R31" s="76" t="s">
         <v>82</v>
       </c>
-      <c r="S31" s="77"/>
-      <c r="T31" s="77" t="s">
+      <c r="S31" s="76"/>
+      <c r="T31" s="76" t="s">
         <v>83</v>
       </c>
-      <c r="U31" s="77"/>
+      <c r="U31" s="76"/>
       <c r="V31" s="9"/>
       <c r="X31" s="5"/>
-      <c r="Y31" s="77" t="s">
+      <c r="Y31" s="76" t="s">
         <v>79</v>
       </c>
-      <c r="Z31" s="77"/>
-      <c r="AA31" s="77" t="s">
+      <c r="Z31" s="76"/>
+      <c r="AA31" s="76" t="s">
         <v>82</v>
       </c>
-      <c r="AB31" s="77"/>
+      <c r="AB31" s="76"/>
       <c r="AC31" s="9"/>
-      <c r="AD31" s="77" t="s">
+      <c r="AD31" s="76" t="s">
         <v>83</v>
       </c>
-      <c r="AE31" s="77"/>
-    </row>
-    <row r="32" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AE31" s="76"/>
+    </row>
+    <row r="32" spans="1:50" x14ac:dyDescent="0.3">
       <c r="P32" s="6" t="s">
         <v>80</v>
       </c>
@@ -13447,7 +14730,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="14:31" x14ac:dyDescent="0.25">
+    <row r="33" spans="14:31" x14ac:dyDescent="0.3">
       <c r="N33" t="s">
         <v>63</v>
       </c>
@@ -13505,7 +14788,7 @@
         <v>6.848409582985554E-2</v>
       </c>
     </row>
-    <row r="34" spans="14:31" x14ac:dyDescent="0.25">
+    <row r="34" spans="14:31" x14ac:dyDescent="0.3">
       <c r="N34" t="s">
         <v>64</v>
       </c>
@@ -13563,7 +14846,7 @@
         <v>4.4728391319122464E-2</v>
       </c>
     </row>
-    <row r="35" spans="14:31" x14ac:dyDescent="0.25">
+    <row r="35" spans="14:31" x14ac:dyDescent="0.3">
       <c r="N35" t="s">
         <v>65</v>
       </c>
@@ -13621,7 +14904,7 @@
         <v>4.0425617308828564E-2</v>
       </c>
     </row>
-    <row r="36" spans="14:31" x14ac:dyDescent="0.25">
+    <row r="36" spans="14:31" x14ac:dyDescent="0.3">
       <c r="N36" s="12" t="s">
         <v>66</v>
       </c>
@@ -13680,7 +14963,7 @@
         <v>3.3078111121048033E-2</v>
       </c>
     </row>
-    <row r="37" spans="14:31" x14ac:dyDescent="0.25">
+    <row r="37" spans="14:31" x14ac:dyDescent="0.3">
       <c r="P37" s="1">
         <f>P36-MAX(P33:P35)</f>
         <v>0.43007095369273662</v>
@@ -13732,7 +15015,7 @@
         <v>-5.4006909946345788E-4</v>
       </c>
     </row>
-    <row r="39" spans="14:31" x14ac:dyDescent="0.25">
+    <row r="39" spans="14:31" x14ac:dyDescent="0.3">
       <c r="N39" s="5" t="s">
         <v>73</v>
       </c>
@@ -13741,38 +15024,38 @@
         <v>74</v>
       </c>
     </row>
-    <row r="40" spans="14:31" x14ac:dyDescent="0.25">
+    <row r="40" spans="14:31" x14ac:dyDescent="0.3">
       <c r="N40" s="5"/>
       <c r="O40" s="5"/>
-      <c r="P40" s="77" t="s">
+      <c r="P40" s="76" t="s">
         <v>79</v>
       </c>
-      <c r="Q40" s="77"/>
-      <c r="R40" s="77" t="s">
+      <c r="Q40" s="76"/>
+      <c r="R40" s="76" t="s">
         <v>82</v>
       </c>
-      <c r="S40" s="77"/>
-      <c r="T40" s="77" t="s">
+      <c r="S40" s="76"/>
+      <c r="T40" s="76" t="s">
         <v>83</v>
       </c>
-      <c r="U40" s="77"/>
+      <c r="U40" s="76"/>
       <c r="V40" s="9"/>
       <c r="X40" s="5"/>
-      <c r="Y40" s="77" t="s">
+      <c r="Y40" s="76" t="s">
         <v>79</v>
       </c>
-      <c r="Z40" s="77"/>
-      <c r="AA40" s="77" t="s">
+      <c r="Z40" s="76"/>
+      <c r="AA40" s="76" t="s">
         <v>82</v>
       </c>
-      <c r="AB40" s="77"/>
+      <c r="AB40" s="76"/>
       <c r="AC40" s="9"/>
-      <c r="AD40" s="77" t="s">
+      <c r="AD40" s="76" t="s">
         <v>83</v>
       </c>
-      <c r="AE40" s="77"/>
-    </row>
-    <row r="41" spans="14:31" x14ac:dyDescent="0.25">
+      <c r="AE40" s="76"/>
+    </row>
+    <row r="41" spans="14:31" x14ac:dyDescent="0.3">
       <c r="P41" s="6" t="s">
         <v>80</v>
       </c>
@@ -13812,7 +15095,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="14:31" x14ac:dyDescent="0.25">
+    <row r="42" spans="14:31" x14ac:dyDescent="0.3">
       <c r="N42" t="s">
         <v>63</v>
       </c>
@@ -13870,7 +15153,7 @@
         <v>5.5886731508572401E-2</v>
       </c>
     </row>
-    <row r="43" spans="14:31" x14ac:dyDescent="0.25">
+    <row r="43" spans="14:31" x14ac:dyDescent="0.3">
       <c r="N43" t="s">
         <v>64</v>
       </c>
@@ -13928,7 +15211,7 @@
         <v>2.3978686559382869E-2</v>
       </c>
     </row>
-    <row r="44" spans="14:31" x14ac:dyDescent="0.25">
+    <row r="44" spans="14:31" x14ac:dyDescent="0.3">
       <c r="N44" t="s">
         <v>65</v>
       </c>
@@ -13986,7 +15269,7 @@
         <v>0.12076274311293005</v>
       </c>
     </row>
-    <row r="45" spans="14:31" x14ac:dyDescent="0.25">
+    <row r="45" spans="14:31" x14ac:dyDescent="0.3">
       <c r="N45" s="12" t="s">
         <v>66</v>
       </c>
@@ -14045,7 +15328,7 @@
         <v>4.7928049947332567E-2</v>
       </c>
     </row>
-    <row r="46" spans="14:31" x14ac:dyDescent="0.25">
+    <row r="46" spans="14:31" x14ac:dyDescent="0.3">
       <c r="P46" s="1">
         <f>P45-MAX(P42:P44)</f>
         <v>0.40952168638386638</v>
@@ -14097,10 +15380,10 @@
         <v>1.7221205626408763E-3</v>
       </c>
     </row>
-    <row r="47" spans="14:31" x14ac:dyDescent="0.25">
+    <row r="47" spans="14:31" x14ac:dyDescent="0.3">
       <c r="P47" s="1"/>
     </row>
-    <row r="48" spans="14:31" x14ac:dyDescent="0.25">
+    <row r="48" spans="14:31" x14ac:dyDescent="0.3">
       <c r="N48" t="s">
         <v>84</v>
       </c>
@@ -14112,7 +15395,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="49" spans="14:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="14:19" x14ac:dyDescent="0.3">
       <c r="R49" s="1">
         <f>AVERAGE(Q37,S37,U37,Z37,AB37,AE37,Q46,S46,U46,Z46,AB46,AE46)</f>
         <v>-1.2476035036042461E-3</v>
@@ -14121,10 +15404,10 @@
         <v>102</v>
       </c>
     </row>
-    <row r="50" spans="14:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="14:19" x14ac:dyDescent="0.3">
       <c r="R50" s="8"/>
     </row>
-    <row r="51" spans="14:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N51" t="s">
         <v>103</v>
       </c>
@@ -14133,7 +15416,7 @@
         <v>0.39663539743408682</v>
       </c>
     </row>
-    <row r="52" spans="14:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="14:19" x14ac:dyDescent="0.3">
       <c r="R52" s="1">
         <f>AVERAGE(Q37,Z37,Q46,Z46)</f>
         <v>-6.246905098322598E-3</v>
@@ -14141,6 +15424,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="AD40:AE40"/>
+    <mergeCell ref="P40:Q40"/>
+    <mergeCell ref="R40:S40"/>
+    <mergeCell ref="T40:U40"/>
+    <mergeCell ref="Y40:Z40"/>
+    <mergeCell ref="AA40:AB40"/>
     <mergeCell ref="P2:T2"/>
     <mergeCell ref="W2:AO2"/>
     <mergeCell ref="D26:D28"/>
@@ -14153,12 +15442,6 @@
     <mergeCell ref="W3:AA3"/>
     <mergeCell ref="AD3:AH3"/>
     <mergeCell ref="AK3:AO3"/>
-    <mergeCell ref="AD40:AE40"/>
-    <mergeCell ref="P40:Q40"/>
-    <mergeCell ref="R40:S40"/>
-    <mergeCell ref="T40:U40"/>
-    <mergeCell ref="Y40:Z40"/>
-    <mergeCell ref="AA40:AB40"/>
   </mergeCells>
   <conditionalFormatting sqref="Y20">
     <cfRule type="cellIs" dxfId="61" priority="52" operator="greaterThan">
@@ -14358,7 +15641,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B866A135-4E8F-4309-AF8D-0270B0ECA943}">
   <dimension ref="B2:R37"/>
   <sheetViews>
@@ -14366,20 +15649,20 @@
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="19.2" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="32" style="14" customWidth="1"/>
-    <col min="3" max="5" width="9.7109375" style="68" customWidth="1"/>
+    <col min="3" max="5" width="9.6640625" style="68" customWidth="1"/>
     <col min="6" max="6" width="2" style="68" customWidth="1"/>
-    <col min="7" max="9" width="9.7109375" style="68" customWidth="1"/>
-    <col min="10" max="10" width="2.7109375" style="68" customWidth="1"/>
-    <col min="11" max="13" width="9.7109375" style="68" customWidth="1"/>
+    <col min="7" max="9" width="9.6640625" style="68" customWidth="1"/>
+    <col min="10" max="10" width="2.6640625" style="68" customWidth="1"/>
+    <col min="11" max="13" width="9.6640625" style="68" customWidth="1"/>
     <col min="14" max="14" width="2" style="68" customWidth="1"/>
-    <col min="15" max="17" width="9.7109375" style="68" customWidth="1"/>
-    <col min="18" max="18" width="2.140625" style="68" customWidth="1"/>
+    <col min="15" max="17" width="9.6640625" style="68" customWidth="1"/>
+    <col min="18" max="18" width="2.109375" style="68" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C2" s="88" t="s">
         <v>66</v>
       </c>
@@ -14403,7 +15686,7 @@
       <c r="P2" s="88"/>
       <c r="Q2" s="88"/>
     </row>
-    <row r="3" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="69" t="s">
         <v>138</v>
       </c>
@@ -14447,7 +15730,7 @@
       </c>
       <c r="R3" s="71"/>
     </row>
-    <row r="4" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="14" t="s">
         <v>140</v>
       </c>
@@ -14491,7 +15774,7 @@
       </c>
       <c r="R4" s="71"/>
     </row>
-    <row r="5" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="14" t="s">
         <v>141</v>
       </c>
@@ -14535,7 +15818,7 @@
       </c>
       <c r="R5" s="71"/>
     </row>
-    <row r="6" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="73" t="s">
         <v>142</v>
       </c>
@@ -14579,7 +15862,7 @@
       </c>
       <c r="R6" s="71"/>
     </row>
-    <row r="7" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="14" t="s">
         <v>118</v>
       </c>
@@ -14623,7 +15906,7 @@
       </c>
       <c r="R7" s="71"/>
     </row>
-    <row r="8" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="14" t="s">
         <v>143</v>
       </c>
@@ -14667,7 +15950,7 @@
       </c>
       <c r="R8" s="71"/>
     </row>
-    <row r="9" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="73" t="s">
         <v>144</v>
       </c>
@@ -14711,7 +15994,7 @@
       </c>
       <c r="R9" s="71"/>
     </row>
-    <row r="10" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="14" t="s">
         <v>119</v>
       </c>
@@ -14755,7 +16038,7 @@
       </c>
       <c r="R10" s="71"/>
     </row>
-    <row r="11" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="14" t="s">
         <v>145</v>
       </c>
@@ -14799,7 +16082,7 @@
       </c>
       <c r="R11" s="71"/>
     </row>
-    <row r="12" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="73" t="s">
         <v>146</v>
       </c>
@@ -14843,7 +16126,7 @@
       </c>
       <c r="R12" s="71"/>
     </row>
-    <row r="13" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="14" t="s">
         <v>120</v>
       </c>
@@ -14887,7 +16170,7 @@
       </c>
       <c r="R13" s="71"/>
     </row>
-    <row r="14" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="14" t="s">
         <v>147</v>
       </c>
@@ -14931,7 +16214,7 @@
       </c>
       <c r="R14" s="71"/>
     </row>
-    <row r="15" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="73" t="s">
         <v>148</v>
       </c>
@@ -14975,7 +16258,7 @@
       </c>
       <c r="R15" s="71"/>
     </row>
-    <row r="16" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="14" t="s">
         <v>149</v>
       </c>
@@ -15019,7 +16302,7 @@
       </c>
       <c r="R16" s="71"/>
     </row>
-    <row r="17" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="14" t="s">
         <v>150</v>
       </c>
@@ -15063,7 +16346,7 @@
       </c>
       <c r="R17" s="71"/>
     </row>
-    <row r="18" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="14" t="s">
         <v>151</v>
       </c>
@@ -15108,7 +16391,7 @@
       </c>
       <c r="R18" s="71"/>
     </row>
-    <row r="21" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="14" t="s">
         <v>152</v>
       </c>
@@ -15122,7 +16405,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="22" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="14" t="s">
         <v>66</v>
       </c>
@@ -15139,7 +16422,7 @@
         <v>0.89922292723442532</v>
       </c>
     </row>
-    <row r="23" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="14" t="s">
         <v>63</v>
       </c>
@@ -15156,7 +16439,7 @@
         <v>0.27932673086955834</v>
       </c>
     </row>
-    <row r="24" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="14" t="s">
         <v>64</v>
       </c>
@@ -15173,7 +16456,7 @@
         <v>0.30156445148128991</v>
       </c>
     </row>
-    <row r="25" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="14" t="s">
         <v>65</v>
       </c>
@@ -15190,7 +16473,7 @@
         <v>2.9512516469038168E-2</v>
       </c>
     </row>
-    <row r="27" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="14" t="s">
         <v>155</v>
       </c>
@@ -15204,7 +16487,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="28" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="14" t="s">
         <v>66</v>
       </c>
@@ -15221,7 +16504,7 @@
         <v>0.85819695891751036</v>
       </c>
     </row>
-    <row r="29" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="14" t="s">
         <v>63</v>
       </c>
@@ -15238,7 +16521,7 @@
         <v>0.37651479525694564</v>
       </c>
     </row>
-    <row r="30" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="14" t="s">
         <v>64</v>
       </c>
@@ -15255,7 +16538,7 @@
         <v>0.21949571194026479</v>
       </c>
     </row>
-    <row r="31" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="14" t="s">
         <v>65</v>
       </c>
@@ -15272,7 +16555,7 @@
         <v>0.22973224280993454</v>
       </c>
     </row>
-    <row r="33" spans="2:5" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="14" t="s">
         <v>156</v>
       </c>
@@ -15286,7 +16569,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="34" spans="2:5" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="14" t="s">
         <v>66</v>
       </c>
@@ -15303,7 +16586,7 @@
         <v>0.7568337337165959</v>
       </c>
     </row>
-    <row r="35" spans="2:5" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="14" t="s">
         <v>63</v>
       </c>
@@ -15320,7 +16603,7 @@
         <v>0.47858368663394896</v>
       </c>
     </row>
-    <row r="36" spans="2:5" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:5" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="14" t="s">
         <v>64</v>
       </c>
@@ -15337,7 +16620,7 @@
         <v>0.58647588269673701</v>
       </c>
     </row>
-    <row r="37" spans="2:5" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:5" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="14" t="s">
         <v>65</v>
       </c>
@@ -15546,28 +16829,28 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C24CE1B-5F25-4F08-AF84-32F62E14361D}">
   <dimension ref="B2:R37"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="19.2" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="31.85546875" style="14" customWidth="1"/>
-    <col min="3" max="5" width="9.7109375" style="68" customWidth="1"/>
+    <col min="2" max="2" width="31.88671875" style="14" customWidth="1"/>
+    <col min="3" max="5" width="9.6640625" style="68" customWidth="1"/>
     <col min="6" max="6" width="2" style="68" customWidth="1"/>
-    <col min="7" max="9" width="9.7109375" style="68" customWidth="1"/>
-    <col min="10" max="10" width="2.7109375" style="68" customWidth="1"/>
-    <col min="11" max="13" width="9.7109375" style="68" customWidth="1"/>
+    <col min="7" max="9" width="9.6640625" style="68" customWidth="1"/>
+    <col min="10" max="10" width="2.6640625" style="68" customWidth="1"/>
+    <col min="11" max="13" width="9.6640625" style="68" customWidth="1"/>
     <col min="14" max="14" width="2" style="68" customWidth="1"/>
-    <col min="15" max="17" width="9.7109375" style="68" customWidth="1"/>
-    <col min="18" max="18" width="2.140625" style="68" customWidth="1"/>
+    <col min="15" max="17" width="9.6640625" style="68" customWidth="1"/>
+    <col min="18" max="18" width="2.109375" style="68" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C2" s="88" t="s">
         <v>66</v>
       </c>
@@ -15591,7 +16874,7 @@
       <c r="P2" s="88"/>
       <c r="Q2" s="88"/>
     </row>
-    <row r="3" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="69" t="s">
         <v>138</v>
       </c>
@@ -15635,7 +16918,7 @@
       </c>
       <c r="R3" s="71"/>
     </row>
-    <row r="4" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="14" t="s">
         <v>140</v>
       </c>
@@ -15679,7 +16962,7 @@
       </c>
       <c r="R4" s="71"/>
     </row>
-    <row r="5" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="14" t="s">
         <v>141</v>
       </c>
@@ -15723,7 +17006,7 @@
       </c>
       <c r="R5" s="71"/>
     </row>
-    <row r="6" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="73" t="s">
         <v>142</v>
       </c>
@@ -15767,7 +17050,7 @@
       </c>
       <c r="R6" s="71"/>
     </row>
-    <row r="7" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="14" t="s">
         <v>118</v>
       </c>
@@ -15811,7 +17094,7 @@
       </c>
       <c r="R7" s="71"/>
     </row>
-    <row r="8" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="14" t="s">
         <v>143</v>
       </c>
@@ -15855,7 +17138,7 @@
       </c>
       <c r="R8" s="71"/>
     </row>
-    <row r="9" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="73" t="s">
         <v>144</v>
       </c>
@@ -15899,7 +17182,7 @@
       </c>
       <c r="R9" s="71"/>
     </row>
-    <row r="10" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="14" t="s">
         <v>119</v>
       </c>
@@ -15943,7 +17226,7 @@
       </c>
       <c r="R10" s="71"/>
     </row>
-    <row r="11" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="14" t="s">
         <v>145</v>
       </c>
@@ -15987,7 +17270,7 @@
       </c>
       <c r="R11" s="71"/>
     </row>
-    <row r="12" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="73" t="s">
         <v>146</v>
       </c>
@@ -16031,7 +17314,7 @@
       </c>
       <c r="R12" s="71"/>
     </row>
-    <row r="13" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="14" t="s">
         <v>120</v>
       </c>
@@ -16075,7 +17358,7 @@
       </c>
       <c r="R13" s="71"/>
     </row>
-    <row r="14" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="14" t="s">
         <v>147</v>
       </c>
@@ -16119,7 +17402,7 @@
       </c>
       <c r="R14" s="71"/>
     </row>
-    <row r="15" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="73" t="s">
         <v>148</v>
       </c>
@@ -16163,7 +17446,7 @@
       </c>
       <c r="R15" s="71"/>
     </row>
-    <row r="16" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="14" t="s">
         <v>149</v>
       </c>
@@ -16207,7 +17490,7 @@
       </c>
       <c r="R16" s="71"/>
     </row>
-    <row r="17" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="14" t="s">
         <v>150</v>
       </c>
@@ -16251,7 +17534,7 @@
       </c>
       <c r="R17" s="71"/>
     </row>
-    <row r="18" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="14" t="s">
         <v>151</v>
       </c>
@@ -16296,7 +17579,7 @@
       </c>
       <c r="R18" s="71"/>
     </row>
-    <row r="21" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="14" t="s">
         <v>152</v>
       </c>
@@ -16310,7 +17593,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="22" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="14" t="s">
         <v>66</v>
       </c>
@@ -16327,7 +17610,7 @@
         <v>0.89491520766354837</v>
       </c>
     </row>
-    <row r="23" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="14" t="s">
         <v>63</v>
       </c>
@@ -16344,7 +17627,7 @@
         <v>0.32367041753362297</v>
       </c>
     </row>
-    <row r="24" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="14" t="s">
         <v>64</v>
       </c>
@@ -16361,7 +17644,7 @@
         <v>0.24241453144546188</v>
       </c>
     </row>
-    <row r="25" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="14" t="s">
         <v>65</v>
       </c>
@@ -16378,7 +17661,7 @@
         <v>0.22788502468652663</v>
       </c>
     </row>
-    <row r="27" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="14" t="s">
         <v>155</v>
       </c>
@@ -16392,7 +17675,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="28" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="14" t="s">
         <v>66</v>
       </c>
@@ -16409,7 +17692,7 @@
         <v>0.83829625874393032</v>
       </c>
     </row>
-    <row r="29" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="14" t="s">
         <v>63</v>
       </c>
@@ -16426,7 +17709,7 @@
         <v>0.37236143413799683</v>
       </c>
     </row>
-    <row r="30" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="14" t="s">
         <v>64</v>
       </c>
@@ -16443,7 +17726,7 @@
         <v>0.53856201574853113</v>
       </c>
     </row>
-    <row r="31" spans="2:18" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="14" t="s">
         <v>65</v>
       </c>
@@ -16460,7 +17743,7 @@
         <v>0.31026329354478949</v>
       </c>
     </row>
-    <row r="33" spans="2:5" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="14" t="s">
         <v>156</v>
       </c>
@@ -16474,7 +17757,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="34" spans="2:5" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="14" t="s">
         <v>66</v>
       </c>
@@ -16491,7 +17774,7 @@
         <v>0.76831972378959135</v>
       </c>
     </row>
-    <row r="35" spans="2:5" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="14" t="s">
         <v>63</v>
       </c>
@@ -16508,7 +17791,7 @@
         <v>0.528375579139723</v>
       </c>
     </row>
-    <row r="36" spans="2:5" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:5" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="14" t="s">
         <v>64</v>
       </c>
@@ -16525,7 +17808,7 @@
         <v>0.68138609510383441</v>
       </c>
     </row>
-    <row r="37" spans="2:5" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:5" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="14" t="s">
         <v>65</v>
       </c>
@@ -16734,43 +18017,42 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5049A103-2C9C-4FAF-AFB0-0228DA8ECD06}">
   <dimension ref="A1:AU51"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O1" sqref="O1:AK1048576"/>
+    <sheetView showGridLines="0" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O32" sqref="O32:T35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="43.5703125" style="14" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="43.5703125" hidden="1" customWidth="1"/>
-    <col min="7" max="10" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" hidden="1" customWidth="1"/>
-    <col min="12" max="13" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="24.140625" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="30" max="30" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="34" max="34" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="36" max="36" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="38" max="38" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="39" max="40" width="9.140625" customWidth="1"/>
+    <col min="1" max="3" width="9.109375" customWidth="1"/>
+    <col min="4" max="4" width="43.5546875" style="14" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" customWidth="1"/>
+    <col min="6" max="6" width="43.5546875" customWidth="1"/>
+    <col min="7" max="10" width="9.109375" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" customWidth="1"/>
+    <col min="12" max="13" width="9.109375" customWidth="1"/>
+    <col min="14" max="14" width="24.109375" customWidth="1"/>
+    <col min="16" max="16" width="9.109375" customWidth="1"/>
+    <col min="17" max="17" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.109375" customWidth="1"/>
+    <col min="20" max="20" width="9.109375" customWidth="1"/>
+    <col min="22" max="22" width="9.109375" customWidth="1"/>
+    <col min="24" max="24" width="9.109375" customWidth="1"/>
+    <col min="26" max="26" width="9.109375" customWidth="1"/>
+    <col min="28" max="28" width="9.109375" customWidth="1"/>
+    <col min="30" max="30" width="9.109375" customWidth="1"/>
+    <col min="32" max="32" width="9.109375" customWidth="1"/>
+    <col min="34" max="34" width="9.109375" customWidth="1"/>
+    <col min="36" max="36" width="9.109375" customWidth="1"/>
+    <col min="38" max="40" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" ht="4.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
       <c r="D2" s="48"/>
       <c r="E2" s="49"/>
       <c r="F2" s="49"/>
@@ -16810,7 +18092,7 @@
       <c r="AJ2" s="82"/>
       <c r="AK2" s="83"/>
     </row>
-    <row r="3" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
@@ -16927,7 +18209,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:47" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
@@ -17047,7 +18329,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:47" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -17167,7 +18449,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:47" s="16" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" s="16" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16">
         <v>2</v>
       </c>
@@ -17294,7 +18576,7 @@
       <c r="AT6"/>
       <c r="AU6"/>
     </row>
-    <row r="7" spans="1:47" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3</v>
       </c>
@@ -17412,7 +18694,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:47" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>4</v>
       </c>
@@ -17530,7 +18812,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:47" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>5</v>
       </c>
@@ -17648,7 +18930,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:47" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>6</v>
       </c>
@@ -17766,7 +19048,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:47" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>7</v>
       </c>
@@ -17884,7 +19166,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:47" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>8</v>
       </c>
@@ -18002,7 +19284,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:47" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:47" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>9</v>
       </c>
@@ -18120,7 +19402,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:47" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:47" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>10</v>
       </c>
@@ -18238,7 +19520,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:47" s="16" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:47" s="16" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16">
         <v>11</v>
       </c>
@@ -18363,7 +19645,7 @@
       <c r="AT15"/>
       <c r="AU15"/>
     </row>
-    <row r="16" spans="1:47" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:47" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>12</v>
       </c>
@@ -18481,7 +19763,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:47" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:47" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>13</v>
       </c>
@@ -18599,7 +19881,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:47" s="4" customFormat="1" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:47" s="4" customFormat="1" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
         <v>14</v>
       </c>
@@ -18724,7 +20006,7 @@
       <c r="AT18"/>
       <c r="AU18"/>
     </row>
-    <row r="19" spans="1:47" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:47" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="D19" s="47" t="s">
         <v>110</v>
       </c>
@@ -18802,7 +20084,7 @@
       <c r="AN19" s="1"/>
       <c r="AP19" s="1"/>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.3">
       <c r="D20" s="52" t="s">
         <v>111</v>
       </c>
@@ -18876,7 +20158,7 @@
         <v>0.31002724777814872</v>
       </c>
     </row>
-    <row r="21" spans="1:47" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:47" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D21" s="15"/>
       <c r="AO21"/>
       <c r="AP21"/>
@@ -18886,8 +20168,8 @@
       <c r="AT21"/>
       <c r="AU21"/>
     </row>
-    <row r="22" spans="1:47" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:47" ht="21" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:47" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:47" ht="21" x14ac:dyDescent="0.4">
       <c r="D24" s="24" t="s">
         <v>109</v>
       </c>
@@ -18993,7 +20275,7 @@
       <c r="AM24" s="2"/>
       <c r="AN24" s="2"/>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.3">
       <c r="D25" s="84" t="s">
         <v>104</v>
       </c>
@@ -19099,7 +20381,7 @@
       <c r="AM25" s="2"/>
       <c r="AN25" s="2"/>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.3">
       <c r="D26" s="84"/>
       <c r="N26" t="s">
         <v>70</v>
@@ -19203,7 +20485,7 @@
       <c r="AM26" s="2"/>
       <c r="AN26" s="2"/>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.3">
       <c r="D27" s="84"/>
       <c r="N27" s="5" t="s">
         <v>68</v>
@@ -19307,7 +20589,7 @@
       <c r="AM27" s="2"/>
       <c r="AN27" s="2"/>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.3">
       <c r="N29" s="5" t="s">
         <v>72</v>
       </c>
@@ -19315,35 +20597,35 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.3">
       <c r="N30" s="5"/>
-      <c r="O30" s="77" t="s">
+      <c r="O30" s="76" t="s">
         <v>79</v>
       </c>
-      <c r="P30" s="77"/>
-      <c r="Q30" s="77" t="s">
+      <c r="P30" s="76"/>
+      <c r="Q30" s="76" t="s">
         <v>82</v>
       </c>
-      <c r="R30" s="77"/>
-      <c r="S30" s="77" t="s">
+      <c r="R30" s="76"/>
+      <c r="S30" s="76" t="s">
         <v>83</v>
       </c>
-      <c r="T30" s="77"/>
+      <c r="T30" s="76"/>
       <c r="V30" s="5"/>
-      <c r="W30" s="77" t="s">
+      <c r="W30" s="76" t="s">
         <v>79</v>
       </c>
-      <c r="X30" s="77"/>
-      <c r="Y30" s="77" t="s">
+      <c r="X30" s="76"/>
+      <c r="Y30" s="76" t="s">
         <v>82</v>
       </c>
-      <c r="Z30" s="77"/>
-      <c r="AA30" s="77" t="s">
+      <c r="Z30" s="76"/>
+      <c r="AA30" s="76" t="s">
         <v>83</v>
       </c>
-      <c r="AB30" s="77"/>
-    </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AB30" s="76"/>
+    </row>
+    <row r="31" spans="1:47" x14ac:dyDescent="0.3">
       <c r="O31" s="6" t="s">
         <v>80</v>
       </c>
@@ -19381,7 +20663,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.3">
       <c r="N32" t="s">
         <v>63</v>
       </c>
@@ -19437,7 +20719,7 @@
         <v>3.8569337851537933E-2</v>
       </c>
     </row>
-    <row r="33" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="33" spans="14:28" x14ac:dyDescent="0.3">
       <c r="N33" t="s">
         <v>64</v>
       </c>
@@ -19493,7 +20775,7 @@
         <v>3.5786645237970267E-2</v>
       </c>
     </row>
-    <row r="34" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="34" spans="14:28" x14ac:dyDescent="0.3">
       <c r="N34" t="s">
         <v>65</v>
       </c>
@@ -19549,7 +20831,7 @@
         <v>0.10950027492948076</v>
       </c>
     </row>
-    <row r="35" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="35" spans="14:28" x14ac:dyDescent="0.3">
       <c r="N35" s="12" t="s">
         <v>66</v>
       </c>
@@ -19605,7 +20887,7 @@
         <v>3.6211908842901132E-2</v>
       </c>
     </row>
-    <row r="36" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="36" spans="14:28" x14ac:dyDescent="0.3">
       <c r="O36" s="1">
         <f>O35-MAX(O32:O34)</f>
         <v>0.33959624716378189</v>
@@ -19655,7 +20937,7 @@
         <v>3.0618364658241155E-5</v>
       </c>
     </row>
-    <row r="38" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="38" spans="14:28" x14ac:dyDescent="0.3">
       <c r="N38" s="5" t="s">
         <v>73</v>
       </c>
@@ -19663,35 +20945,35 @@
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="39" spans="14:28" x14ac:dyDescent="0.3">
       <c r="N39" s="5"/>
-      <c r="O39" s="77" t="s">
+      <c r="O39" s="76" t="s">
         <v>79</v>
       </c>
-      <c r="P39" s="77"/>
-      <c r="Q39" s="77" t="s">
+      <c r="P39" s="76"/>
+      <c r="Q39" s="76" t="s">
         <v>82</v>
       </c>
-      <c r="R39" s="77"/>
-      <c r="S39" s="77" t="s">
+      <c r="R39" s="76"/>
+      <c r="S39" s="76" t="s">
         <v>83</v>
       </c>
-      <c r="T39" s="77"/>
+      <c r="T39" s="76"/>
       <c r="V39" s="5"/>
-      <c r="W39" s="77" t="s">
+      <c r="W39" s="76" t="s">
         <v>79</v>
       </c>
-      <c r="X39" s="77"/>
-      <c r="Y39" s="77" t="s">
+      <c r="X39" s="76"/>
+      <c r="Y39" s="76" t="s">
         <v>82</v>
       </c>
-      <c r="Z39" s="77"/>
-      <c r="AA39" s="77" t="s">
+      <c r="Z39" s="76"/>
+      <c r="AA39" s="76" t="s">
         <v>83</v>
       </c>
-      <c r="AB39" s="77"/>
-    </row>
-    <row r="40" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="AB39" s="76"/>
+    </row>
+    <row r="40" spans="14:28" x14ac:dyDescent="0.3">
       <c r="O40" s="6" t="s">
         <v>80</v>
       </c>
@@ -19729,7 +21011,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="41" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="41" spans="14:28" x14ac:dyDescent="0.3">
       <c r="N41" t="s">
         <v>63</v>
       </c>
@@ -19785,7 +21067,7 @@
         <v>6.6615746659743028E-2</v>
       </c>
     </row>
-    <row r="42" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="42" spans="14:28" x14ac:dyDescent="0.3">
       <c r="N42" t="s">
         <v>64</v>
       </c>
@@ -19841,7 +21123,7 @@
         <v>1.7139106622392833E-2</v>
       </c>
     </row>
-    <row r="43" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="43" spans="14:28" x14ac:dyDescent="0.3">
       <c r="N43" t="s">
         <v>65</v>
       </c>
@@ -19897,7 +21179,7 @@
         <v>9.7060296902856294E-2</v>
       </c>
     </row>
-    <row r="44" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="44" spans="14:28" x14ac:dyDescent="0.3">
       <c r="N44" s="12" t="s">
         <v>66</v>
       </c>
@@ -19953,7 +21235,7 @@
         <v>5.3278268527140765E-2</v>
       </c>
     </row>
-    <row r="45" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="45" spans="14:28" x14ac:dyDescent="0.3">
       <c r="O45" s="1">
         <f>O44-MAX(O41:O43)</f>
         <v>0.28402103680849899</v>
@@ -20003,10 +21285,10 @@
         <v>2.544824921436368E-3</v>
       </c>
     </row>
-    <row r="46" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="46" spans="14:28" x14ac:dyDescent="0.3">
       <c r="O46" s="1"/>
     </row>
-    <row r="47" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="47" spans="14:28" x14ac:dyDescent="0.3">
       <c r="N47" t="s">
         <v>84</v>
       </c>
@@ -20018,7 +21300,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="14:28" x14ac:dyDescent="0.25">
+    <row r="48" spans="14:28" x14ac:dyDescent="0.3">
       <c r="Q48" s="1">
         <f>AVERAGE(P36,R36,T36,X36,Z36,AB36,P45,R45,T45,X45,Z45,AB45)</f>
         <v>-3.2894540640592625E-5</v>
@@ -20027,10 +21309,10 @@
         <v>102</v>
       </c>
     </row>
-    <row r="49" spans="14:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="14:17" x14ac:dyDescent="0.3">
       <c r="Q49" s="8"/>
     </row>
-    <row r="50" spans="14:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="14:17" x14ac:dyDescent="0.3">
       <c r="N50" t="s">
         <v>103</v>
       </c>
@@ -20039,7 +21321,7 @@
         <v>0.35730121535000026</v>
       </c>
     </row>
-    <row r="51" spans="14:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="14:17" x14ac:dyDescent="0.3">
       <c r="Q51" s="1">
         <f>AVERAGE(P36,X36,P45,X45)</f>
         <v>-3.9206223618157392E-3</v>

</xml_diff>